<commit_message>
add the Vokss.xlsx file
</commit_message>
<xml_diff>
--- a/VOKSS прейскурант_ 2.xlsx
+++ b/VOKSS прейскурант_ 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="розподіл матеріалів (Fabric)" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="392">
   <si>
     <t xml:space="preserve">Примерное распределение материалов по группам сложности в зависимости от трудоѐмкости обработки</t>
   </si>
@@ -37,9 +37,18 @@
     <t xml:space="preserve">Группа 0</t>
   </si>
   <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coplexity factor = 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Шѐлковый бархат</t>
   </si>
   <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ткани со сплошным застилом бисером</t>
   </si>
   <si>
@@ -338,6 +347,9 @@
   </si>
   <si>
     <t xml:space="preserve">Женская одежда (часть I)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fabric.coplexity_factor</t>
   </si>
   <si>
     <t xml:space="preserve">Наименование изделия</t>
@@ -1839,10 +1851,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:B35"/>
+  <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1861,160 +1873,169 @@
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2048,387 +2069,387 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2450,7 +2471,7 @@
   <dimension ref="B2:M78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2458,7 +2479,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="60.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="69.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="26.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="7" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="8.53"/>
@@ -2468,37 +2489,40 @@
   <sheetData>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="10" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="16" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D4" s="18" t="n">
         <v>1</v>
@@ -2521,7 +2545,7 @@
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="16"/>
       <c r="C5" s="20" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D5" s="18" t="n">
         <v>2</v>
@@ -2539,10 +2563,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="16" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D6" s="18" t="n">
         <v>1</v>
@@ -2565,7 +2589,7 @@
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="16"/>
       <c r="C7" s="20" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D7" s="18" t="n">
         <v>2</v>
@@ -2584,7 +2608,7 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="16"/>
       <c r="C8" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D8" s="18" t="n">
         <v>3</v>
@@ -2606,10 +2630,10 @@
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="16" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D9" s="18" t="n">
         <v>1</v>
@@ -2632,7 +2656,7 @@
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="16"/>
       <c r="C10" s="20" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D10" s="18" t="n">
         <v>2</v>
@@ -2651,7 +2675,7 @@
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="16"/>
       <c r="C11" s="20" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D11" s="18" t="n">
         <v>3</v>
@@ -2670,7 +2694,7 @@
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="16"/>
       <c r="C12" s="20" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D12" s="18" t="n">
         <v>4</v>
@@ -2688,10 +2712,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="16" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D13" s="18" t="n">
         <v>1</v>
@@ -2710,7 +2734,7 @@
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="16"/>
       <c r="C14" s="20" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D14" s="18" t="n">
         <v>2</v>
@@ -2729,7 +2753,7 @@
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="16"/>
       <c r="C15" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D15" s="18" t="n">
         <v>3</v>
@@ -2747,10 +2771,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="16" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D16" s="18" t="n">
         <v>1</v>
@@ -2769,7 +2793,7 @@
     <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="16"/>
       <c r="C17" s="20" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D17" s="18" t="n">
         <v>2</v>
@@ -2788,7 +2812,7 @@
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="16"/>
       <c r="C18" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D18" s="18" t="n">
         <v>3</v>
@@ -2806,10 +2830,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="16" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D19" s="18" t="n">
         <v>1</v>
@@ -2828,7 +2852,7 @@
     <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="16"/>
       <c r="C20" s="20" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D20" s="18" t="n">
         <v>2</v>
@@ -2847,7 +2871,7 @@
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="16"/>
       <c r="C21" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D21" s="18" t="n">
         <v>3</v>
@@ -2865,10 +2889,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>121</v>
       </c>
       <c r="D22" s="18" t="n">
         <v>1</v>
@@ -2887,7 +2911,7 @@
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="16"/>
       <c r="C23" s="20" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D23" s="18" t="n">
         <v>2</v>
@@ -2906,7 +2930,7 @@
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="16"/>
       <c r="C24" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D24" s="18" t="n">
         <v>3</v>
@@ -2924,10 +2948,10 @@
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="16" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D25" s="18" t="n">
         <v>2</v>
@@ -2946,7 +2970,7 @@
     <row r="26" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="16"/>
       <c r="C26" s="20" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D26" s="18" t="n">
         <v>3</v>
@@ -2964,10 +2988,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="16" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D27" s="18" t="n">
         <v>1</v>
@@ -2986,7 +3010,7 @@
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="16"/>
       <c r="C28" s="20" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D28" s="18" t="n">
         <v>2</v>
@@ -3005,7 +3029,7 @@
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="16"/>
       <c r="C29" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D29" s="18" t="n">
         <v>3</v>
@@ -3023,10 +3047,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="16" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D30" s="18" t="n">
         <v>1</v>
@@ -3045,7 +3069,7 @@
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="16"/>
       <c r="C31" s="20" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D31" s="18" t="n">
         <v>2</v>
@@ -3064,7 +3088,7 @@
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="16"/>
       <c r="C32" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D32" s="18" t="n">
         <v>3</v>
@@ -3082,10 +3106,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="16" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D33" s="18" t="n">
         <v>1</v>
@@ -3104,7 +3128,7 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="16"/>
       <c r="C34" s="20" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D34" s="18" t="n">
         <v>2</v>
@@ -3119,7 +3143,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="16"/>
       <c r="C35" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D35" s="18" t="n">
         <v>3</v>
@@ -3133,10 +3157,10 @@
     </row>
     <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="16" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D36" s="18" t="n">
         <v>2</v>
@@ -3150,10 +3174,10 @@
     </row>
     <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="16" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="19" t="n">
@@ -3165,10 +3189,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="16" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D38" s="18" t="n">
         <v>1</v>
@@ -3183,7 +3207,7 @@
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="16"/>
       <c r="C39" s="20" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D39" s="18" t="n">
         <v>2</v>
@@ -3198,7 +3222,7 @@
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="16"/>
       <c r="C40" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D40" s="18" t="n">
         <v>3</v>
@@ -3212,10 +3236,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="16" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D41" s="18" t="n">
         <v>1</v>
@@ -3230,7 +3254,7 @@
     <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="16"/>
       <c r="C42" s="20" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D42" s="18" t="n">
         <v>2</v>
@@ -3245,7 +3269,7 @@
     <row r="43" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="16"/>
       <c r="C43" s="20" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D43" s="18" t="n">
         <v>3</v>
@@ -3259,10 +3283,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="16" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D44" s="18" t="n">
         <v>1</v>
@@ -3277,7 +3301,7 @@
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="16"/>
       <c r="C45" s="20" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D45" s="18" t="n">
         <v>2</v>
@@ -3292,7 +3316,7 @@
     <row r="46" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="16"/>
       <c r="C46" s="20" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D46" s="18" t="n">
         <v>3</v>
@@ -3306,10 +3330,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="16" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D47" s="18" t="n">
         <v>1</v>
@@ -3324,7 +3348,7 @@
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="16"/>
       <c r="C48" s="20" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D48" s="18" t="n">
         <v>2</v>
@@ -3339,7 +3363,7 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="16"/>
       <c r="C49" s="20" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D49" s="18" t="n">
         <v>3</v>
@@ -3353,10 +3377,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="16" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D50" s="18"/>
       <c r="E50" s="19" t="n">
@@ -3369,7 +3393,7 @@
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="16"/>
       <c r="C51" s="20" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D51" s="18"/>
       <c r="E51" s="19" t="n">
@@ -3382,7 +3406,7 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="16"/>
       <c r="C52" s="20" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D52" s="18"/>
       <c r="E52" s="19" t="n">
@@ -3394,10 +3418,10 @@
     </row>
     <row r="53" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="21" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D53" s="18" t="n">
         <v>1</v>
@@ -3412,7 +3436,7 @@
     <row r="54" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="21"/>
       <c r="C54" s="20" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D54" s="18" t="n">
         <v>2</v>
@@ -3427,7 +3451,7 @@
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="21"/>
       <c r="C55" s="20" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D55" s="18" t="n">
         <v>3</v>
@@ -3442,7 +3466,7 @@
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="21"/>
       <c r="C56" s="20" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D56" s="18" t="n">
         <v>4</v>
@@ -3456,10 +3480,10 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="21" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D57" s="18" t="n">
         <v>1</v>
@@ -3474,7 +3498,7 @@
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="21"/>
       <c r="C58" s="20" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D58" s="18" t="n">
         <v>2</v>
@@ -3489,7 +3513,7 @@
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="21"/>
       <c r="C59" s="20" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D59" s="18" t="n">
         <v>3</v>
@@ -3504,7 +3528,7 @@
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="21"/>
       <c r="C60" s="20" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D60" s="18" t="n">
         <v>4</v>
@@ -3518,10 +3542,10 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="21" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D61" s="18" t="n">
         <v>2</v>
@@ -3536,7 +3560,7 @@
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="21"/>
       <c r="C62" s="20" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D62" s="18" t="n">
         <v>3</v>
@@ -3551,7 +3575,7 @@
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="21"/>
       <c r="C63" s="20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D63" s="18" t="n">
         <v>4</v>
@@ -3565,10 +3589,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="21" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D64" s="18" t="n">
         <v>2</v>
@@ -3583,10 +3607,10 @@
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="21"/>
       <c r="C65" s="20" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E65" s="22" t="n">
         <v>150</v>
@@ -3597,10 +3621,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="21" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D66" s="18" t="n">
         <v>2</v>
@@ -3615,10 +3639,10 @@
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="21"/>
       <c r="C67" s="20" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E67" s="22" t="n">
         <v>72.5</v>
@@ -3681,10 +3705,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3701,7 +3725,7 @@
     </row>
     <row r="2" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -3709,13 +3733,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D3" s="26"/>
     </row>
@@ -3731,7 +3755,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B5" s="29" t="n">
         <v>1</v>
@@ -3758,7 +3782,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="28"/>
       <c r="B7" s="31" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C7" s="32" t="n">
         <v>25.1301775147929</v>
@@ -3769,7 +3793,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="28" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B8" s="29" t="n">
         <v>1</v>
@@ -3796,7 +3820,7 @@
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="28"/>
       <c r="B10" s="31" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C10" s="32" t="n">
         <v>20.1041420118343</v>
@@ -3807,7 +3831,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="33" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B11" s="34" t="n">
         <v>1</v>
@@ -3821,7 +3845,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="36" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B12" s="37" t="n">
         <v>2</v>
@@ -3835,10 +3859,10 @@
     </row>
     <row r="13" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="39" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C13" s="41" t="n">
         <v>20</v>
@@ -3847,7 +3871,11 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="6">
@@ -3875,7 +3903,7 @@
   </sheetPr>
   <dimension ref="A2:E117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -3892,39 +3920,39 @@
   <sheetData>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="45" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D2" s="46"/>
     </row>
     <row r="3" s="50" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="47" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="51" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B4" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E4" s="54" t="n">
         <v>1</v>
@@ -3935,7 +3963,7 @@
       <c r="B5" s="21"/>
       <c r="C5" s="52"/>
       <c r="D5" s="53" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E5" s="54" t="n">
         <v>1</v>
@@ -3946,7 +3974,7 @@
       <c r="B6" s="21"/>
       <c r="C6" s="52"/>
       <c r="D6" s="53" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E6" s="54" t="n">
         <v>1</v>
@@ -3957,7 +3985,7 @@
       <c r="B7" s="21"/>
       <c r="C7" s="52"/>
       <c r="D7" s="53" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E7" s="54" t="n">
         <v>2</v>
@@ -3969,10 +3997,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E8" s="54" t="n">
         <v>1</v>
@@ -3984,10 +4012,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E9" s="54" t="n">
         <v>1</v>
@@ -3998,7 +4026,7 @@
       <c r="B10" s="18"/>
       <c r="C10" s="52"/>
       <c r="D10" s="20" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E10" s="54" t="n">
         <v>1</v>
@@ -4009,7 +4037,7 @@
       <c r="B11" s="18"/>
       <c r="C11" s="52"/>
       <c r="D11" s="20" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>1</v>
@@ -4020,7 +4048,7 @@
       <c r="B12" s="18"/>
       <c r="C12" s="52"/>
       <c r="D12" s="20" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>1</v>
@@ -4031,7 +4059,7 @@
       <c r="B13" s="18"/>
       <c r="C13" s="52"/>
       <c r="D13" s="20" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>1</v>
@@ -4043,10 +4071,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>2</v>
@@ -4058,10 +4086,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D15" s="52" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E15" s="16" t="n">
         <v>1</v>
@@ -4073,10 +4101,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E16" s="16" t="n">
         <v>1</v>
@@ -4087,7 +4115,7 @@
       <c r="B17" s="21"/>
       <c r="C17" s="16"/>
       <c r="D17" s="52" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E17" s="16" t="n">
         <v>1</v>
@@ -4098,7 +4126,7 @@
       <c r="B18" s="21"/>
       <c r="C18" s="16"/>
       <c r="D18" s="52" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E18" s="16" t="n">
         <v>1</v>
@@ -4106,16 +4134,16 @@
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="51" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B19" s="18" t="n">
         <v>7</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E19" s="16" t="n">
         <v>1</v>
@@ -4127,10 +4155,10 @@
         <v>8</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E20" s="55" t="n">
         <v>1</v>
@@ -4142,10 +4170,10 @@
         <v>9</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E21" s="16" t="n">
         <v>4</v>
@@ -4157,10 +4185,10 @@
         <v>10</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E22" s="55" t="n">
         <v>1</v>
@@ -4172,10 +4200,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E23" s="55" t="n">
         <v>1</v>
@@ -4187,10 +4215,10 @@
         <v>12</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E24" s="55" t="n">
         <v>1</v>
@@ -4201,7 +4229,7 @@
       <c r="B25" s="21"/>
       <c r="C25" s="16"/>
       <c r="D25" s="52" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E25" s="55" t="n">
         <v>1</v>
@@ -4209,16 +4237,16 @@
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="51" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B26" s="18" t="n">
         <v>13</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E26" s="54"/>
     </row>
@@ -4227,7 +4255,7 @@
       <c r="B27" s="18"/>
       <c r="C27" s="16"/>
       <c r="D27" s="52" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E27" s="55" t="n">
         <v>1</v>
@@ -4238,7 +4266,7 @@
       <c r="B28" s="18"/>
       <c r="C28" s="16"/>
       <c r="D28" s="20" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E28" s="55" t="n">
         <v>1</v>
@@ -4249,7 +4277,7 @@
       <c r="B29" s="18"/>
       <c r="C29" s="16"/>
       <c r="D29" s="20" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E29" s="55" t="n">
         <v>1</v>
@@ -4260,7 +4288,7 @@
       <c r="B30" s="18"/>
       <c r="C30" s="16"/>
       <c r="D30" s="20" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E30" s="55" t="n">
         <v>1</v>
@@ -4271,7 +4299,7 @@
       <c r="B31" s="18"/>
       <c r="C31" s="16"/>
       <c r="D31" s="20" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E31" s="55" t="n">
         <v>1</v>
@@ -4282,7 +4310,7 @@
       <c r="B32" s="18"/>
       <c r="C32" s="16"/>
       <c r="D32" s="20" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E32" s="55" t="n">
         <v>1</v>
@@ -4294,10 +4322,10 @@
         <v>14</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E33" s="55" t="n">
         <v>1</v>
@@ -4309,10 +4337,10 @@
         <v>15</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E34" s="55" t="n">
         <v>1</v>
@@ -4324,10 +4352,10 @@
         <v>16</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E35" s="55" t="n">
         <v>2</v>
@@ -4338,7 +4366,7 @@
       <c r="B36" s="21"/>
       <c r="C36" s="16"/>
       <c r="D36" s="20" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E36" s="55" t="n">
         <v>2</v>
@@ -4350,10 +4378,10 @@
         <v>17</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E37" s="55" t="n">
         <v>4</v>
@@ -4361,16 +4389,16 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="51" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B38" s="21" t="n">
         <v>18</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E38" s="54"/>
     </row>
@@ -4379,7 +4407,7 @@
       <c r="B39" s="21"/>
       <c r="C39" s="16"/>
       <c r="D39" s="20" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E39" s="55" t="n">
         <v>1</v>
@@ -4390,7 +4418,7 @@
       <c r="B40" s="21"/>
       <c r="C40" s="16"/>
       <c r="D40" s="20" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E40" s="55" t="n">
         <v>1</v>
@@ -4402,10 +4430,10 @@
         <v>19</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E41" s="55" t="n">
         <v>1</v>
@@ -4416,7 +4444,7 @@
       <c r="B42" s="21"/>
       <c r="C42" s="16"/>
       <c r="D42" s="20" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E42" s="55" t="n">
         <v>1</v>
@@ -4428,10 +4456,10 @@
         <v>20</v>
       </c>
       <c r="C43" s="52" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E43" s="55" t="n">
         <v>1</v>
@@ -4443,10 +4471,10 @@
         <v>21</v>
       </c>
       <c r="C44" s="52" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E44" s="55" t="n">
         <v>1</v>
@@ -4454,16 +4482,16 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="51" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B45" s="18" t="n">
         <v>22</v>
       </c>
       <c r="C45" s="52" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E45" s="54" t="n">
         <v>1</v>
@@ -4475,10 +4503,10 @@
         <v>23</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E46" s="55" t="n">
         <v>2</v>
@@ -4489,7 +4517,7 @@
       <c r="B47" s="21"/>
       <c r="C47" s="16"/>
       <c r="D47" s="20" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E47" s="55" t="n">
         <v>2</v>
@@ -4500,7 +4528,7 @@
       <c r="B48" s="21"/>
       <c r="C48" s="16"/>
       <c r="D48" s="20" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="E48" s="55" t="n">
         <v>1</v>
@@ -4512,7 +4540,7 @@
         <v>24</v>
       </c>
       <c r="C49" s="52" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="55" t="n">
@@ -4525,10 +4553,10 @@
         <v>25</v>
       </c>
       <c r="C50" s="52" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D50" s="52" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E50" s="55" t="n">
         <v>1</v>
@@ -4540,10 +4568,10 @@
         <v>26</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D51" s="52" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E51" s="55" t="n">
         <v>2</v>
@@ -4555,7 +4583,7 @@
         <v>27</v>
       </c>
       <c r="C52" s="52" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="55" t="n">
@@ -4568,10 +4596,10 @@
         <v>28</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E53" s="55" t="n">
         <v>4</v>
@@ -4583,7 +4611,7 @@
         <v>29</v>
       </c>
       <c r="C54" s="52" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D54" s="20"/>
       <c r="E54" s="55" t="n">
@@ -4596,10 +4624,10 @@
         <v>30</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D55" s="52" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="E55" s="55" t="n">
         <v>1</v>
@@ -4611,10 +4639,10 @@
         <v>31</v>
       </c>
       <c r="C56" s="52" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D56" s="52" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E56" s="55" t="n">
         <v>2</v>
@@ -4626,7 +4654,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="52" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="55" t="n">
@@ -4639,10 +4667,10 @@
         <v>33</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="E58" s="55" t="n">
         <v>2</v>
@@ -4650,16 +4678,16 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="51" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B59" s="18" t="n">
         <v>34</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D59" s="52" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E59" s="55"/>
     </row>
@@ -4668,7 +4696,7 @@
       <c r="B60" s="18"/>
       <c r="C60" s="16"/>
       <c r="D60" s="52" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E60" s="55" t="n">
         <v>1</v>
@@ -4679,7 +4707,7 @@
       <c r="B61" s="18"/>
       <c r="C61" s="16"/>
       <c r="D61" s="52" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E61" s="55" t="n">
         <v>1</v>
@@ -4690,7 +4718,7 @@
       <c r="B62" s="18"/>
       <c r="C62" s="16"/>
       <c r="D62" s="52" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="E62" s="55" t="n">
         <v>1</v>
@@ -4701,7 +4729,7 @@
       <c r="B63" s="18"/>
       <c r="C63" s="16"/>
       <c r="D63" s="52" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E63" s="55" t="n">
         <v>1</v>
@@ -4713,10 +4741,10 @@
         <v>35</v>
       </c>
       <c r="C64" s="52" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D64" s="52" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E64" s="55" t="n">
         <v>2</v>
@@ -4728,10 +4756,10 @@
         <v>36</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D65" s="52" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E65" s="54"/>
     </row>
@@ -4740,7 +4768,7 @@
       <c r="B66" s="21"/>
       <c r="C66" s="16"/>
       <c r="D66" s="52" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E66" s="55" t="n">
         <v>1</v>
@@ -4751,7 +4779,7 @@
       <c r="B67" s="21"/>
       <c r="C67" s="16"/>
       <c r="D67" s="52" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E67" s="55" t="n">
         <v>1</v>
@@ -4763,10 +4791,10 @@
         <v>37</v>
       </c>
       <c r="C68" s="52" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D68" s="52" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="E68" s="55" t="n">
         <v>1</v>
@@ -4774,16 +4802,16 @@
     </row>
     <row r="69" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="51" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B69" s="18" t="n">
         <v>38</v>
       </c>
       <c r="C69" s="52" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D69" s="52" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E69" s="55" t="n">
         <v>1</v>
@@ -4795,10 +4823,10 @@
         <v>39</v>
       </c>
       <c r="C70" s="52" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E70" s="55" t="n">
         <v>2</v>
@@ -4810,10 +4838,10 @@
         <v>40</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D71" s="52" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E71" s="55" t="n">
         <v>2</v>
@@ -4825,10 +4853,10 @@
         <v>41</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D72" s="52" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="E72" s="55" t="n">
         <v>1</v>
@@ -4839,7 +4867,7 @@
       <c r="B73" s="18"/>
       <c r="C73" s="16"/>
       <c r="D73" s="52" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E73" s="55" t="n">
         <v>1</v>
@@ -4850,7 +4878,7 @@
       <c r="B74" s="18"/>
       <c r="C74" s="16"/>
       <c r="D74" s="52" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E74" s="55" t="n">
         <v>1</v>
@@ -4861,7 +4889,7 @@
       <c r="B75" s="18"/>
       <c r="C75" s="16"/>
       <c r="D75" s="52" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="E75" s="55" t="n">
         <v>1</v>
@@ -4872,7 +4900,7 @@
       <c r="B76" s="18"/>
       <c r="C76" s="16"/>
       <c r="D76" s="52" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E76" s="55" t="n">
         <v>1</v>
@@ -4883,7 +4911,7 @@
       <c r="B77" s="18"/>
       <c r="C77" s="16"/>
       <c r="D77" s="52" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E77" s="55" t="n">
         <v>1</v>
@@ -4895,10 +4923,10 @@
         <v>42</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E78" s="55" t="n">
         <v>1</v>
@@ -4909,7 +4937,7 @@
       <c r="B79" s="18"/>
       <c r="C79" s="16"/>
       <c r="D79" s="20" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="E79" s="55" t="n">
         <v>1</v>
@@ -4920,7 +4948,7 @@
       <c r="B80" s="18"/>
       <c r="C80" s="16"/>
       <c r="D80" s="20" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E80" s="55" t="n">
         <v>1</v>
@@ -4931,7 +4959,7 @@
       <c r="B81" s="18"/>
       <c r="C81" s="16"/>
       <c r="D81" s="20" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E81" s="55" t="n">
         <v>1</v>
@@ -4942,7 +4970,7 @@
       <c r="B82" s="18"/>
       <c r="C82" s="16"/>
       <c r="D82" s="20" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E82" s="55" t="n">
         <v>1</v>
@@ -4953,7 +4981,7 @@
       <c r="B83" s="18"/>
       <c r="C83" s="16"/>
       <c r="D83" s="20" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="E83" s="55" t="n">
         <v>1</v>
@@ -4965,10 +4993,10 @@
         <v>43</v>
       </c>
       <c r="C84" s="52" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D84" s="20" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="E84" s="55" t="n">
         <v>2</v>
@@ -4980,7 +5008,7 @@
         <v>44</v>
       </c>
       <c r="C85" s="52" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D85" s="20"/>
       <c r="E85" s="55" t="n">
@@ -4989,13 +5017,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="51" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B86" s="18" t="n">
         <v>45</v>
       </c>
       <c r="C86" s="52" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D86" s="20"/>
       <c r="E86" s="55" t="n">
@@ -5008,7 +5036,7 @@
         <v>46</v>
       </c>
       <c r="C87" s="52" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D87" s="20"/>
       <c r="E87" s="55" t="n">
@@ -5021,7 +5049,7 @@
         <v>47</v>
       </c>
       <c r="C88" s="52" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="D88" s="20"/>
       <c r="E88" s="55" t="n">
@@ -5034,10 +5062,10 @@
         <v>48</v>
       </c>
       <c r="C89" s="52" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D89" s="20" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="E89" s="55" t="n">
         <v>1</v>
@@ -5049,7 +5077,7 @@
         <v>49</v>
       </c>
       <c r="C90" s="52" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="D90" s="20"/>
       <c r="E90" s="55" t="n">
@@ -5062,10 +5090,10 @@
         <v>50</v>
       </c>
       <c r="C91" s="52" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E91" s="55" t="n">
         <v>2</v>
@@ -5073,16 +5101,16 @@
     </row>
     <row r="92" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="51" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B92" s="18" t="n">
         <v>51</v>
       </c>
       <c r="C92" s="52" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="D92" s="20" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="E92" s="54" t="n">
         <v>4</v>
@@ -5094,10 +5122,10 @@
         <v>52</v>
       </c>
       <c r="C93" s="52" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D93" s="20" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E93" s="54" t="n">
         <v>1</v>
@@ -5109,7 +5137,7 @@
         <v>53</v>
       </c>
       <c r="C94" s="52" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D94" s="20"/>
       <c r="E94" s="54" t="n">
@@ -5122,7 +5150,7 @@
         <v>54</v>
       </c>
       <c r="C95" s="52" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D95" s="20"/>
       <c r="E95" s="54" t="n">
@@ -5135,10 +5163,10 @@
         <v>55</v>
       </c>
       <c r="C96" s="52" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D96" s="20" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="E96" s="54" t="n">
         <v>1</v>
@@ -5150,10 +5178,10 @@
         <v>56</v>
       </c>
       <c r="C97" s="52" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E97" s="54" t="n">
         <v>1</v>
@@ -5165,10 +5193,10 @@
         <v>57</v>
       </c>
       <c r="C98" s="52" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="E98" s="54" t="n">
         <v>1</v>
@@ -5180,10 +5208,10 @@
         <v>58</v>
       </c>
       <c r="C99" s="52" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E99" s="54" t="n">
         <v>1</v>
@@ -5195,7 +5223,7 @@
         <v>59</v>
       </c>
       <c r="C100" s="52" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="D100" s="20"/>
       <c r="E100" s="54" t="n">
@@ -5208,7 +5236,7 @@
         <v>60</v>
       </c>
       <c r="C101" s="52" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D101" s="20"/>
       <c r="E101" s="54" t="n">
@@ -5221,10 +5249,10 @@
         <v>61</v>
       </c>
       <c r="C102" s="16" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D102" s="20" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="E102" s="54" t="n">
         <v>1</v>
@@ -5235,7 +5263,7 @@
       <c r="B103" s="21"/>
       <c r="C103" s="16"/>
       <c r="D103" s="20" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E103" s="54" t="n">
         <v>1</v>
@@ -5246,7 +5274,7 @@
       <c r="B104" s="21"/>
       <c r="C104" s="16"/>
       <c r="D104" s="20" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="E104" s="54" t="n">
         <v>1</v>
@@ -5257,7 +5285,7 @@
       <c r="B105" s="21"/>
       <c r="C105" s="16"/>
       <c r="D105" s="20" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E105" s="54" t="n">
         <v>1</v>
@@ -5269,10 +5297,10 @@
         <v>62</v>
       </c>
       <c r="C106" s="16" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="D106" s="20" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="E106" s="54" t="n">
         <v>1</v>
@@ -5283,7 +5311,7 @@
       <c r="B107" s="18"/>
       <c r="C107" s="16"/>
       <c r="D107" s="20" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="E107" s="54" t="n">
         <v>1</v>
@@ -5294,7 +5322,7 @@
       <c r="B108" s="18"/>
       <c r="C108" s="16"/>
       <c r="D108" s="20" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="E108" s="54" t="n">
         <v>1</v>
@@ -5305,7 +5333,7 @@
       <c r="B109" s="18"/>
       <c r="C109" s="16"/>
       <c r="D109" s="20" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="E109" s="54" t="n">
         <v>1</v>
@@ -5316,7 +5344,7 @@
       <c r="B110" s="18"/>
       <c r="C110" s="16"/>
       <c r="D110" s="20" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="E110" s="54" t="n">
         <v>1</v>
@@ -5327,7 +5355,7 @@
       <c r="B111" s="18"/>
       <c r="C111" s="16"/>
       <c r="D111" s="20" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E111" s="54" t="n">
         <v>1</v>
@@ -5339,7 +5367,7 @@
         <v>63</v>
       </c>
       <c r="C112" s="52" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D112" s="20"/>
       <c r="E112" s="54" t="n">
@@ -5352,7 +5380,7 @@
         <v>64</v>
       </c>
       <c r="C113" s="52" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D113" s="20"/>
       <c r="E113" s="54" t="n">
@@ -5365,7 +5393,7 @@
         <v>65</v>
       </c>
       <c r="C114" s="52" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D114" s="20"/>
       <c r="E114" s="54" t="n">
@@ -5378,7 +5406,7 @@
         <v>66</v>
       </c>
       <c r="C115" s="52" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="D115" s="20"/>
       <c r="E115" s="54" t="n">
@@ -5391,7 +5419,7 @@
         <v>67</v>
       </c>
       <c r="C116" s="52" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="D116" s="20"/>
       <c r="E116" s="54" t="n">
@@ -5404,7 +5432,7 @@
         <v>68</v>
       </c>
       <c r="C117" s="52" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D117" s="20"/>
       <c r="E117" s="54" t="n">
@@ -5470,7 +5498,7 @@
   </sheetPr>
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -5486,7 +5514,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="57" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C2" s="57"/>
       <c r="D2" s="57"/>
@@ -5494,41 +5522,41 @@
     <row r="3" s="6" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="58"/>
       <c r="B3" s="48" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="58" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B4" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="D4" s="59" t="n">
         <v>0.2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="52" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B5" s="21" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D5" s="59" t="n">
         <v>0.2</v>
@@ -5538,7 +5566,7 @@
       <c r="A6" s="52"/>
       <c r="B6" s="21"/>
       <c r="C6" s="60" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D6" s="61" t="n">
         <v>0.15</v>
@@ -5546,13 +5574,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="62" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B7" s="21" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D7" s="61" t="n">
         <v>0.3</v>
@@ -5562,7 +5590,7 @@
       <c r="A8" s="62"/>
       <c r="B8" s="21"/>
       <c r="C8" s="60" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D8" s="61" t="n">
         <v>0.15</v>
@@ -5572,7 +5600,7 @@
       <c r="A9" s="62"/>
       <c r="B9" s="21"/>
       <c r="C9" s="60" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="D9" s="61" t="n">
         <v>0.15</v>
@@ -5580,13 +5608,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="62" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B10" s="21" t="n">
         <v>4</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D10" s="61" t="n">
         <v>-0.3</v>
@@ -5596,7 +5624,7 @@
       <c r="A11" s="62"/>
       <c r="B11" s="21"/>
       <c r="C11" s="60" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D11" s="61" t="n">
         <v>-0.3</v>
@@ -5604,13 +5632,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="62" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B12" s="21" t="n">
         <v>5</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D12" s="61" t="n">
         <v>0.3</v>
@@ -5620,7 +5648,7 @@
       <c r="A13" s="62"/>
       <c r="B13" s="21"/>
       <c r="C13" s="60" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D13" s="61" t="n">
         <v>0.4</v>
@@ -5630,7 +5658,7 @@
       <c r="A14" s="62"/>
       <c r="B14" s="21"/>
       <c r="C14" s="60" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D14" s="61" t="n">
         <v>0.4</v>
@@ -5681,7 +5709,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="63" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5689,110 +5717,110 @@
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="64" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="64" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C5" s="64"/>
       <c r="D5" s="65" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="64"/>
       <c r="C6" s="64"/>
       <c r="D6" s="65" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="64"/>
       <c r="C7" s="64"/>
       <c r="D7" s="65" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="64"/>
       <c r="C8" s="64"/>
       <c r="D8" s="65" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="64"/>
       <c r="C9" s="64"/>
       <c r="D9" s="65" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="64"/>
       <c r="C10" s="64"/>
       <c r="D10" s="65" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="64" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="64" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="64" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="C13" s="65" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="64" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C14" s="64"/>
       <c r="D14" s="66" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="67"/>
     </row>
     <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="68" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="C15" s="68"/>
       <c r="D15" s="69" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
create a lot of .html :) edit some models etc...
</commit_message>
<xml_diff>
--- a/VOKSS прейскурант_ 2.xlsx
+++ b/VOKSS прейскурант_ 2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="401">
   <si>
     <t xml:space="preserve">Примерное распределение материалов по группам сложности в зависимости от трудоѐмкости обработки</t>
   </si>
@@ -591,14 +591,18 @@
   </si>
   <si>
     <t xml:space="preserve">Наименование
-усложняющих эл-тов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дополнительные характеристики усложняющих элементов</t>
+усложняющих эл-тов (group)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дополнительные характеристики усложняющих элементов (name)</t>
   </si>
   <si>
     <t xml:space="preserve">Кол-во
-усл. элем. (складність)</t>
+усл. элем. (complexity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">базова ціна ускладнюючого елемента
+(base_price)</t>
   </si>
   <si>
     <t xml:space="preserve">Рельефы, швы, складки, клинья, шлицы (разрезы)</t>
@@ -1156,223 +1160,43 @@
     <t xml:space="preserve">надбавка на великий розмір</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- верхняя одежда (включая юбку, брюки, шорты и т.п.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> с полуобхватом груди третьим свыше 58 см. Поясные изделия: для мужчин с полуобхватом талии свыше 56 см, для женщин с полуобхватом бѐдер свыше 62 см:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> - лѐгкая одежда </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> с полуобхватом груди третьим свыше 58 см. Поясные изделия: для мужчин с полуобхватом талии свыше 56 см, для женщин с полуобхватом бѐдер свыше 62 см:</t>
-    </r>
+    <t xml:space="preserve">- верхняя одежда (включая юбку, брюки, шорты и т.п.) с полуобхватом груди третьим свыше 58 см. Поясные изделия: для мужчин с полуобхватом талии свыше 56 см, для женщин с полуобхватом бѐдер свыше 62 см:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - лѐгкая одежда  с полуобхватом груди третьим свыше 58 см. Поясные изделия: для мужчин с полуобхватом талии свыше 56 см, для женщин с полуобхватом бѐдер свыше 62 см:</t>
   </si>
   <si>
     <t xml:space="preserve">Удлинѐнные изделия:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Удлинѐнные изделия:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> платье, халат, юбки и т.п. длиной ниже уровня коленей более 20 см</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Удлинѐнные изделия:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> пальто длиной ниже уровня коленей более 20 см</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Удлинѐнные изделия:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> пиджак, жакет, жилет и т.п. длиной ниже линии бѐдер более 15 см и до коленей</t>
-    </r>
+    <t xml:space="preserve">Удлинѐнные изделия: платье, халат, юбки и т.п. длиной ниже уровня коленей более 20 см</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Удлинѐнные изделия: пальто длиной ниже уровня коленей более 20 см</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Удлинѐнные изделия: пиджак, жакет, жилет и т.п. длиной ниже линии бѐдер более 15 см и до коленей</t>
   </si>
   <si>
     <t xml:space="preserve">Укороченные изделия:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Укороченные изделия::</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> жакет, жилет, куртка длиной до линии талии или выше (кроме жилета под пиджак, фрак, смокинг)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Укороченные изделия:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> полукомбинезон с короткими брюками</t>
-    </r>
+    <t xml:space="preserve">Укороченные изделия:: жакет, жилет, куртка длиной до линии талии или выше (кроме жилета под пиджак, фрак, смокинг)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Укороченные изделия: полукомбинезон с короткими брюками</t>
   </si>
   <si>
     <t xml:space="preserve">Надбавки за срочность:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Надбавки за срочность:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> изготовление мужской и женской верхней одежды (кроме брюк и юбок) в срок до 10 суток</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Надбавки за срочность:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> изготовление мужской и женской лѐгкой одежды, юбок. Брюк, корсетных изделий в срок до 5 суток</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Надбавки за срочность:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> изготовление мужских брюк в срок до 3 суток</t>
-    </r>
+    <t xml:space="preserve">Надбавки за срочность: изготовление мужской и женской верхней одежды (кроме брюк и юбок) в срок до 10 суток</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Надбавки за срочность: изготовление мужской и женской лѐгкой одежды, юбок. Брюк, корсетных изделий в срок до 5 суток</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Надбавки за срочность: изготовление мужских брюк в срок до 3 суток</t>
   </si>
   <si>
     <t xml:space="preserve">Особенности расчета
@@ -1465,7 +1289,7 @@
     <numFmt numFmtId="168" formatCode="D\-MMM"/>
     <numFmt numFmtId="169" formatCode="0%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1534,12 +1358,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1713,7 +1531,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1946,8 +1764,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2030,10 +1848,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2071,10 +1885,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2158,7 +1968,7 @@
   <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2166,7 +1976,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="89.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -4226,7 +4036,7 @@
   <dimension ref="A2:F117"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4246,7 +4056,7 @@
       </c>
       <c r="D2" s="54"/>
     </row>
-    <row r="3" s="59" customFormat="true" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="59" customFormat="true" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="55" t="s">
         <v>179</v>
       </c>
@@ -4263,21 +4073,21 @@
         <v>183</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="60" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B4" s="27" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E4" s="63" t="n">
         <v>1</v>
@@ -4289,7 +4099,7 @@
       <c r="B5" s="27"/>
       <c r="C5" s="61"/>
       <c r="D5" s="62" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E5" s="63" t="n">
         <v>1</v>
@@ -4301,7 +4111,7 @@
       <c r="B6" s="27"/>
       <c r="C6" s="61"/>
       <c r="D6" s="62" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E6" s="63" t="n">
         <v>1</v>
@@ -4313,7 +4123,7 @@
       <c r="B7" s="27"/>
       <c r="C7" s="61"/>
       <c r="D7" s="62" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E7" s="63" t="n">
         <v>2</v>
@@ -4326,10 +4136,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E8" s="63" t="n">
         <v>1</v>
@@ -4342,10 +4152,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E9" s="63" t="n">
         <v>1</v>
@@ -4357,7 +4167,7 @@
       <c r="B10" s="24"/>
       <c r="C10" s="61"/>
       <c r="D10" s="26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E10" s="63" t="n">
         <v>1</v>
@@ -4369,7 +4179,7 @@
       <c r="B11" s="24"/>
       <c r="C11" s="61"/>
       <c r="D11" s="26" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E11" s="63" t="n">
         <v>1</v>
@@ -4381,7 +4191,7 @@
       <c r="B12" s="24"/>
       <c r="C12" s="61"/>
       <c r="D12" s="26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E12" s="63" t="n">
         <v>1</v>
@@ -4393,7 +4203,7 @@
       <c r="B13" s="24"/>
       <c r="C13" s="61"/>
       <c r="D13" s="26" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E13" s="63" t="n">
         <v>1</v>
@@ -4406,10 +4216,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E14" s="63" t="n">
         <v>2</v>
@@ -4422,10 +4232,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E15" s="22" t="n">
         <v>1</v>
@@ -4438,10 +4248,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E16" s="22" t="n">
         <v>1</v>
@@ -4453,7 +4263,7 @@
       <c r="B17" s="27"/>
       <c r="C17" s="22"/>
       <c r="D17" s="61" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E17" s="22" t="n">
         <v>1</v>
@@ -4465,7 +4275,7 @@
       <c r="B18" s="27"/>
       <c r="C18" s="22"/>
       <c r="D18" s="61" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E18" s="22" t="n">
         <v>1</v>
@@ -4474,16 +4284,16 @@
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="60" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B19" s="24" t="n">
         <v>7</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E19" s="22" t="n">
         <v>1</v>
@@ -4496,10 +4306,10 @@
         <v>8</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E20" s="65" t="n">
         <v>1</v>
@@ -4512,10 +4322,10 @@
         <v>9</v>
       </c>
       <c r="C21" s="61" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E21" s="22" t="n">
         <v>4</v>
@@ -4528,10 +4338,10 @@
         <v>10</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E22" s="65" t="n">
         <v>1</v>
@@ -4544,10 +4354,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E23" s="65" t="n">
         <v>1</v>
@@ -4560,10 +4370,10 @@
         <v>12</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D24" s="61" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E24" s="65" t="n">
         <v>1</v>
@@ -4575,7 +4385,7 @@
       <c r="B25" s="27"/>
       <c r="C25" s="22"/>
       <c r="D25" s="61" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E25" s="65" t="n">
         <v>1</v>
@@ -4584,16 +4394,16 @@
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="60" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B26" s="24" t="n">
         <v>13</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E26" s="63"/>
       <c r="F26" s="64"/>
@@ -4603,7 +4413,7 @@
       <c r="B27" s="24"/>
       <c r="C27" s="22"/>
       <c r="D27" s="61" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E27" s="65" t="n">
         <v>1</v>
@@ -4615,7 +4425,7 @@
       <c r="B28" s="24"/>
       <c r="C28" s="22"/>
       <c r="D28" s="26" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E28" s="65" t="n">
         <v>1</v>
@@ -4627,7 +4437,7 @@
       <c r="B29" s="24"/>
       <c r="C29" s="22"/>
       <c r="D29" s="26" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E29" s="65" t="n">
         <v>1</v>
@@ -4639,7 +4449,7 @@
       <c r="B30" s="24"/>
       <c r="C30" s="22"/>
       <c r="D30" s="26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E30" s="65" t="n">
         <v>1</v>
@@ -4651,7 +4461,7 @@
       <c r="B31" s="24"/>
       <c r="C31" s="22"/>
       <c r="D31" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E31" s="65" t="n">
         <v>1</v>
@@ -4663,7 +4473,7 @@
       <c r="B32" s="24"/>
       <c r="C32" s="22"/>
       <c r="D32" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E32" s="65" t="n">
         <v>1</v>
@@ -4676,10 +4486,10 @@
         <v>14</v>
       </c>
       <c r="C33" s="61" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E33" s="65" t="n">
         <v>1</v>
@@ -4692,10 +4502,10 @@
         <v>15</v>
       </c>
       <c r="C34" s="61" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E34" s="65" t="n">
         <v>1</v>
@@ -4708,10 +4518,10 @@
         <v>16</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E35" s="65" t="n">
         <v>2</v>
@@ -4723,7 +4533,7 @@
       <c r="B36" s="27"/>
       <c r="C36" s="22"/>
       <c r="D36" s="26" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E36" s="65" t="n">
         <v>2</v>
@@ -4736,10 +4546,10 @@
         <v>17</v>
       </c>
       <c r="C37" s="61" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E37" s="65" t="n">
         <v>4</v>
@@ -4748,16 +4558,16 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="60" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B38" s="27" t="n">
         <v>18</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E38" s="63"/>
       <c r="F38" s="64"/>
@@ -4767,7 +4577,7 @@
       <c r="B39" s="27"/>
       <c r="C39" s="22"/>
       <c r="D39" s="26" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E39" s="65" t="n">
         <v>1</v>
@@ -4779,7 +4589,7 @@
       <c r="B40" s="27"/>
       <c r="C40" s="22"/>
       <c r="D40" s="26" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E40" s="65" t="n">
         <v>1</v>
@@ -4792,10 +4602,10 @@
         <v>19</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E41" s="65" t="n">
         <v>1</v>
@@ -4807,7 +4617,7 @@
       <c r="B42" s="27"/>
       <c r="C42" s="22"/>
       <c r="D42" s="26" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E42" s="65" t="n">
         <v>1</v>
@@ -4820,10 +4630,10 @@
         <v>20</v>
       </c>
       <c r="C43" s="61" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E43" s="65" t="n">
         <v>1</v>
@@ -4836,10 +4646,10 @@
         <v>21</v>
       </c>
       <c r="C44" s="61" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E44" s="65" t="n">
         <v>1</v>
@@ -4848,16 +4658,16 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="60" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B45" s="24" t="n">
         <v>22</v>
       </c>
       <c r="C45" s="61" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E45" s="63" t="n">
         <v>1</v>
@@ -4870,10 +4680,10 @@
         <v>23</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E46" s="65" t="n">
         <v>2</v>
@@ -4885,7 +4695,7 @@
       <c r="B47" s="27"/>
       <c r="C47" s="22"/>
       <c r="D47" s="26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E47" s="65" t="n">
         <v>2</v>
@@ -4897,7 +4707,7 @@
       <c r="B48" s="27"/>
       <c r="C48" s="22"/>
       <c r="D48" s="26" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E48" s="65" t="n">
         <v>1</v>
@@ -4910,7 +4720,7 @@
         <v>24</v>
       </c>
       <c r="C49" s="61" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D49" s="26"/>
       <c r="E49" s="65" t="n">
@@ -4924,10 +4734,10 @@
         <v>25</v>
       </c>
       <c r="C50" s="61" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D50" s="61" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E50" s="65" t="n">
         <v>1</v>
@@ -4940,10 +4750,10 @@
         <v>26</v>
       </c>
       <c r="C51" s="61" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D51" s="61" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E51" s="65" t="n">
         <v>2</v>
@@ -4956,7 +4766,7 @@
         <v>27</v>
       </c>
       <c r="C52" s="61" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D52" s="26"/>
       <c r="E52" s="65" t="n">
@@ -4970,10 +4780,10 @@
         <v>28</v>
       </c>
       <c r="C53" s="61" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E53" s="65" t="n">
         <v>4</v>
@@ -4986,7 +4796,7 @@
         <v>29</v>
       </c>
       <c r="C54" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="65" t="n">
@@ -5000,10 +4810,10 @@
         <v>30</v>
       </c>
       <c r="C55" s="61" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D55" s="61" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E55" s="65" t="n">
         <v>1</v>
@@ -5016,10 +4826,10 @@
         <v>31</v>
       </c>
       <c r="C56" s="61" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D56" s="61" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E56" s="65" t="n">
         <v>2</v>
@@ -5032,7 +4842,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="61" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="65" t="n">
@@ -5046,10 +4856,10 @@
         <v>33</v>
       </c>
       <c r="C58" s="61" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D58" s="61" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E58" s="65" t="n">
         <v>2</v>
@@ -5058,16 +4868,16 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="60" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B59" s="24" t="n">
         <v>34</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D59" s="61" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E59" s="65"/>
       <c r="F59" s="64"/>
@@ -5077,7 +4887,7 @@
       <c r="B60" s="24"/>
       <c r="C60" s="22"/>
       <c r="D60" s="61" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E60" s="65" t="n">
         <v>1</v>
@@ -5089,7 +4899,7 @@
       <c r="B61" s="24"/>
       <c r="C61" s="22"/>
       <c r="D61" s="61" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E61" s="65" t="n">
         <v>1</v>
@@ -5101,7 +4911,7 @@
       <c r="B62" s="24"/>
       <c r="C62" s="22"/>
       <c r="D62" s="61" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E62" s="65" t="n">
         <v>1</v>
@@ -5113,7 +4923,7 @@
       <c r="B63" s="24"/>
       <c r="C63" s="22"/>
       <c r="D63" s="61" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E63" s="65" t="n">
         <v>1</v>
@@ -5126,10 +4936,10 @@
         <v>35</v>
       </c>
       <c r="C64" s="61" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D64" s="61" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E64" s="65" t="n">
         <v>2</v>
@@ -5142,10 +4952,10 @@
         <v>36</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D65" s="61" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E65" s="63"/>
       <c r="F65" s="64"/>
@@ -5155,7 +4965,7 @@
       <c r="B66" s="27"/>
       <c r="C66" s="22"/>
       <c r="D66" s="61" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E66" s="65" t="n">
         <v>1</v>
@@ -5167,7 +4977,7 @@
       <c r="B67" s="27"/>
       <c r="C67" s="22"/>
       <c r="D67" s="61" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E67" s="65" t="n">
         <v>1</v>
@@ -5180,10 +4990,10 @@
         <v>37</v>
       </c>
       <c r="C68" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D68" s="61" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E68" s="65" t="n">
         <v>1</v>
@@ -5192,16 +5002,16 @@
     </row>
     <row r="69" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="60" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B69" s="24" t="n">
         <v>38</v>
       </c>
       <c r="C69" s="61" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D69" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E69" s="65" t="n">
         <v>1</v>
@@ -5214,10 +5024,10 @@
         <v>39</v>
       </c>
       <c r="C70" s="61" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E70" s="65" t="n">
         <v>2</v>
@@ -5230,10 +5040,10 @@
         <v>40</v>
       </c>
       <c r="C71" s="61" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D71" s="61" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E71" s="65" t="n">
         <v>2</v>
@@ -5246,10 +5056,10 @@
         <v>41</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D72" s="61" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E72" s="65" t="n">
         <v>1</v>
@@ -5261,7 +5071,7 @@
       <c r="B73" s="24"/>
       <c r="C73" s="22"/>
       <c r="D73" s="61" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E73" s="65" t="n">
         <v>1</v>
@@ -5273,7 +5083,7 @@
       <c r="B74" s="24"/>
       <c r="C74" s="22"/>
       <c r="D74" s="61" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E74" s="65" t="n">
         <v>1</v>
@@ -5285,7 +5095,7 @@
       <c r="B75" s="24"/>
       <c r="C75" s="22"/>
       <c r="D75" s="61" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E75" s="65" t="n">
         <v>1</v>
@@ -5297,7 +5107,7 @@
       <c r="B76" s="24"/>
       <c r="C76" s="22"/>
       <c r="D76" s="61" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E76" s="65" t="n">
         <v>1</v>
@@ -5309,7 +5119,7 @@
       <c r="B77" s="24"/>
       <c r="C77" s="22"/>
       <c r="D77" s="61" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E77" s="65" t="n">
         <v>1</v>
@@ -5322,10 +5132,10 @@
         <v>42</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E78" s="65" t="n">
         <v>1</v>
@@ -5337,7 +5147,7 @@
       <c r="B79" s="24"/>
       <c r="C79" s="22"/>
       <c r="D79" s="26" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E79" s="65" t="n">
         <v>1</v>
@@ -5349,7 +5159,7 @@
       <c r="B80" s="24"/>
       <c r="C80" s="22"/>
       <c r="D80" s="26" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E80" s="65" t="n">
         <v>1</v>
@@ -5361,7 +5171,7 @@
       <c r="B81" s="24"/>
       <c r="C81" s="22"/>
       <c r="D81" s="26" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E81" s="65" t="n">
         <v>1</v>
@@ -5373,7 +5183,7 @@
       <c r="B82" s="24"/>
       <c r="C82" s="22"/>
       <c r="D82" s="26" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E82" s="65" t="n">
         <v>1</v>
@@ -5385,7 +5195,7 @@
       <c r="B83" s="24"/>
       <c r="C83" s="22"/>
       <c r="D83" s="26" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E83" s="65" t="n">
         <v>1</v>
@@ -5398,10 +5208,10 @@
         <v>43</v>
       </c>
       <c r="C84" s="61" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E84" s="65" t="n">
         <v>2</v>
@@ -5414,7 +5224,7 @@
         <v>44</v>
       </c>
       <c r="C85" s="61" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D85" s="26"/>
       <c r="E85" s="65" t="n">
@@ -5424,13 +5234,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="60" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B86" s="24" t="n">
         <v>45</v>
       </c>
       <c r="C86" s="61" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D86" s="26"/>
       <c r="E86" s="65" t="n">
@@ -5444,7 +5254,7 @@
         <v>46</v>
       </c>
       <c r="C87" s="61" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D87" s="26"/>
       <c r="E87" s="65" t="n">
@@ -5458,7 +5268,7 @@
         <v>47</v>
       </c>
       <c r="C88" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D88" s="26"/>
       <c r="E88" s="65" t="n">
@@ -5472,10 +5282,10 @@
         <v>48</v>
       </c>
       <c r="C89" s="61" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E89" s="65" t="n">
         <v>1</v>
@@ -5488,7 +5298,7 @@
         <v>49</v>
       </c>
       <c r="C90" s="61" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D90" s="26"/>
       <c r="E90" s="65" t="n">
@@ -5502,10 +5312,10 @@
         <v>50</v>
       </c>
       <c r="C91" s="61" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E91" s="65" t="n">
         <v>2</v>
@@ -5514,16 +5324,16 @@
     </row>
     <row r="92" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="60" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B92" s="24" t="n">
         <v>51</v>
       </c>
       <c r="C92" s="61" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E92" s="63" t="n">
         <v>4</v>
@@ -5536,10 +5346,10 @@
         <v>52</v>
       </c>
       <c r="C93" s="61" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E93" s="63" t="n">
         <v>1</v>
@@ -5552,7 +5362,7 @@
         <v>53</v>
       </c>
       <c r="C94" s="61" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D94" s="26"/>
       <c r="E94" s="63" t="n">
@@ -5566,7 +5376,7 @@
         <v>54</v>
       </c>
       <c r="C95" s="61" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D95" s="26"/>
       <c r="E95" s="63" t="n">
@@ -5580,10 +5390,10 @@
         <v>55</v>
       </c>
       <c r="C96" s="61" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E96" s="63" t="n">
         <v>1</v>
@@ -5596,10 +5406,10 @@
         <v>56</v>
       </c>
       <c r="C97" s="61" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E97" s="63" t="n">
         <v>1</v>
@@ -5612,10 +5422,10 @@
         <v>57</v>
       </c>
       <c r="C98" s="61" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E98" s="63" t="n">
         <v>1</v>
@@ -5628,10 +5438,10 @@
         <v>58</v>
       </c>
       <c r="C99" s="61" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E99" s="63" t="n">
         <v>1</v>
@@ -5644,7 +5454,7 @@
         <v>59</v>
       </c>
       <c r="C100" s="61" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D100" s="26"/>
       <c r="E100" s="63" t="n">
@@ -5658,7 +5468,7 @@
         <v>60</v>
       </c>
       <c r="C101" s="61" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D101" s="26"/>
       <c r="E101" s="63" t="n">
@@ -5672,10 +5482,10 @@
         <v>61</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E102" s="63" t="n">
         <v>1</v>
@@ -5687,7 +5497,7 @@
       <c r="B103" s="27"/>
       <c r="C103" s="22"/>
       <c r="D103" s="26" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E103" s="63" t="n">
         <v>1</v>
@@ -5699,7 +5509,7 @@
       <c r="B104" s="27"/>
       <c r="C104" s="22"/>
       <c r="D104" s="26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E104" s="63" t="n">
         <v>1</v>
@@ -5711,7 +5521,7 @@
       <c r="B105" s="27"/>
       <c r="C105" s="22"/>
       <c r="D105" s="26" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E105" s="63" t="n">
         <v>1</v>
@@ -5724,10 +5534,10 @@
         <v>62</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E106" s="63" t="n">
         <v>1</v>
@@ -5739,7 +5549,7 @@
       <c r="B107" s="24"/>
       <c r="C107" s="22"/>
       <c r="D107" s="26" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E107" s="63" t="n">
         <v>1</v>
@@ -5751,7 +5561,7 @@
       <c r="B108" s="24"/>
       <c r="C108" s="22"/>
       <c r="D108" s="26" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E108" s="63" t="n">
         <v>1</v>
@@ -5763,7 +5573,7 @@
       <c r="B109" s="24"/>
       <c r="C109" s="22"/>
       <c r="D109" s="26" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E109" s="63" t="n">
         <v>1</v>
@@ -5775,7 +5585,7 @@
       <c r="B110" s="24"/>
       <c r="C110" s="22"/>
       <c r="D110" s="26" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E110" s="63" t="n">
         <v>1</v>
@@ -5787,7 +5597,7 @@
       <c r="B111" s="24"/>
       <c r="C111" s="22"/>
       <c r="D111" s="26" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E111" s="63" t="n">
         <v>1</v>
@@ -5800,7 +5610,7 @@
         <v>63</v>
       </c>
       <c r="C112" s="61" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D112" s="26"/>
       <c r="E112" s="63" t="n">
@@ -5814,7 +5624,7 @@
         <v>64</v>
       </c>
       <c r="C113" s="61" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D113" s="26"/>
       <c r="E113" s="63" t="n">
@@ -5828,7 +5638,7 @@
         <v>65</v>
       </c>
       <c r="C114" s="61" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D114" s="26"/>
       <c r="E114" s="63" t="n">
@@ -5842,7 +5652,7 @@
         <v>66</v>
       </c>
       <c r="C115" s="61" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D115" s="26"/>
       <c r="E115" s="63" t="n">
@@ -5856,7 +5666,7 @@
         <v>67</v>
       </c>
       <c r="C116" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D116" s="26"/>
       <c r="E116" s="63" t="n">
@@ -5870,7 +5680,7 @@
         <v>68</v>
       </c>
       <c r="C117" s="61" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D117" s="26"/>
       <c r="E117" s="63" t="n">
@@ -5938,7 +5748,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5953,54 +5763,54 @@
   <sheetData>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="67" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C2" s="67"/>
       <c r="D2" s="67"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="68" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="71" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B4" s="24" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D4" s="72" t="n">
         <v>0.2</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="73" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B5" s="74" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D5" s="72" t="n">
         <v>0.2</v>
@@ -6013,7 +5823,7 @@
       <c r="A6" s="73"/>
       <c r="B6" s="74"/>
       <c r="C6" s="75" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D6" s="77" t="n">
         <v>0.15</v>
@@ -6024,13 +5834,13 @@
     </row>
     <row r="7" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="78" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B7" s="74" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="79" t="s">
-        <v>366</v>
+      <c r="C7" s="75" t="s">
+        <v>367</v>
       </c>
       <c r="D7" s="77" t="n">
         <v>0.3</v>
@@ -6042,8 +5852,8 @@
     <row r="8" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="78"/>
       <c r="B8" s="74"/>
-      <c r="C8" s="79" t="s">
-        <v>367</v>
+      <c r="C8" s="75" t="s">
+        <v>368</v>
       </c>
       <c r="D8" s="77" t="n">
         <v>0.15</v>
@@ -6055,8 +5865,8 @@
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="78"/>
       <c r="B9" s="74"/>
-      <c r="C9" s="79" t="s">
-        <v>368</v>
+      <c r="C9" s="75" t="s">
+        <v>369</v>
       </c>
       <c r="D9" s="77" t="n">
         <v>0.15</v>
@@ -6067,13 +5877,13 @@
     </row>
     <row r="10" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="78" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B10" s="74" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="79" t="s">
-        <v>370</v>
+      <c r="C10" s="75" t="s">
+        <v>371</v>
       </c>
       <c r="D10" s="77" t="n">
         <v>-0.3</v>
@@ -6085,8 +5895,8 @@
     <row r="11" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="78"/>
       <c r="B11" s="74"/>
-      <c r="C11" s="79" t="s">
-        <v>371</v>
+      <c r="C11" s="75" t="s">
+        <v>372</v>
       </c>
       <c r="D11" s="77" t="n">
         <v>-0.3</v>
@@ -6097,13 +5907,13 @@
     </row>
     <row r="12" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="78" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B12" s="74" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="79" t="s">
-        <v>373</v>
+      <c r="C12" s="75" t="s">
+        <v>374</v>
       </c>
       <c r="D12" s="77" t="n">
         <v>0.3</v>
@@ -6115,8 +5925,8 @@
     <row r="13" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="78"/>
       <c r="B13" s="74"/>
-      <c r="C13" s="79" t="s">
-        <v>374</v>
+      <c r="C13" s="75" t="s">
+        <v>375</v>
       </c>
       <c r="D13" s="77" t="n">
         <v>0.4</v>
@@ -6128,8 +5938,8 @@
     <row r="14" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="78"/>
       <c r="B14" s="74"/>
-      <c r="C14" s="79" t="s">
-        <v>375</v>
+      <c r="C14" s="75" t="s">
+        <v>376</v>
       </c>
       <c r="D14" s="77" t="n">
         <v>0.4</v>
@@ -6173,128 +5983,128 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="80" width="4.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="81" width="31.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="81" width="50.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="82" width="138.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="80" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="80" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="79" width="4.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="80" width="31.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="80" width="50.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="81" width="138.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="79" width="8.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="79" width="8.53"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="69.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="83" t="s">
-        <v>376</v>
+      <c r="D2" s="82" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="83"/>
+      <c r="D3" s="82"/>
     </row>
     <row r="4" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="84" t="s">
-        <v>377</v>
-      </c>
-      <c r="C4" s="84" t="s">
+      <c r="B4" s="83" t="s">
         <v>378</v>
       </c>
-      <c r="D4" s="85" t="s">
+      <c r="C4" s="83" t="s">
         <v>379</v>
       </c>
+      <c r="D4" s="84" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="84" t="s">
-        <v>380</v>
-      </c>
-      <c r="C5" s="84"/>
-      <c r="D5" s="85" t="s">
+      <c r="B5" s="83" t="s">
         <v>381</v>
       </c>
+      <c r="C5" s="83"/>
+      <c r="D5" s="84" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="85" t="s">
-        <v>382</v>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="85" t="s">
-        <v>383</v>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="84" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="85" t="s">
-        <v>384</v>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="84" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="85" t="s">
-        <v>385</v>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="84" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="85" t="s">
-        <v>386</v>
+      <c r="B10" s="83"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="84" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="84" t="s">
-        <v>387</v>
-      </c>
-      <c r="C11" s="84" t="s">
+      <c r="B11" s="83" t="s">
         <v>388</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="C11" s="83" t="s">
         <v>389</v>
       </c>
+      <c r="D11" s="84" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="84" t="s">
-        <v>390</v>
-      </c>
-      <c r="C12" s="84" t="s">
+      <c r="B12" s="83" t="s">
         <v>391</v>
       </c>
-      <c r="D12" s="85" t="s">
+      <c r="C12" s="83" t="s">
         <v>392</v>
       </c>
+      <c r="D12" s="84" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="84" t="s">
-        <v>393</v>
-      </c>
-      <c r="C13" s="85" t="s">
+      <c r="B13" s="83" t="s">
         <v>394</v>
       </c>
-      <c r="D13" s="85" t="s">
+      <c r="C13" s="84" t="s">
         <v>395</v>
       </c>
+      <c r="D13" s="84" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="84" t="s">
-        <v>396</v>
-      </c>
-      <c r="C14" s="84"/>
-      <c r="D14" s="86" t="s">
+      <c r="B14" s="83" t="s">
         <v>397</v>
       </c>
-      <c r="E14" s="87"/>
-      <c r="F14" s="88"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="85" t="s">
+        <v>398</v>
+      </c>
+      <c r="E14" s="86"/>
+      <c r="F14" s="87"/>
     </row>
     <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="89"/>
-      <c r="C15" s="90" t="s">
-        <v>398</v>
-      </c>
-      <c r="D15" s="83" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="88" t="s">
         <v>399</v>
+      </c>
+      <c r="D15" s="82" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all models are chenged need to migrate once more
</commit_message>
<xml_diff>
--- a/VOKSS прейскурант_ 2.xlsx
+++ b/VOKSS прейскурант_ 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="розподіл матеріалів (Fabric)" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="401">
   <si>
     <t xml:space="preserve">Примерное распределение материалов по группам сложности в зависимости от трудоѐмкости обработки</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">Платье, сарафан, халат, жакет, блузка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group</t>
   </si>
   <si>
     <t xml:space="preserve">С цельнокроеным станом, прямого или полуприлегающего силуэта, незначительно расклешѐнного по боковым швам (расклешение до 10 см по низу в сложенном вдвое изделии до уровня коленей и до 20 см – в изделии длиной ниже уровня коленей), со средним швом или складкой за счѐт припуска или вставки на переде и на спинке.</t>
@@ -2157,7 +2160,7 @@
   </sheetPr>
   <dimension ref="B2:D35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2372,10 +2375,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:B78"/>
+  <dimension ref="B1:C78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2399,375 +2402,381 @@
       <c r="B4" s="9" t="s">
         <v>39</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2807,40 +2816,40 @@
   <sheetData>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L3" s="21"/>
       <c r="M3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D4" s="24" t="n">
         <v>1</v>
@@ -2863,7 +2872,7 @@
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="22"/>
       <c r="C5" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D5" s="24" t="n">
         <v>2</v>
@@ -2881,10 +2890,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D6" s="24" t="n">
         <v>1</v>
@@ -2907,7 +2916,7 @@
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="22"/>
       <c r="C7" s="26" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D7" s="24" t="n">
         <v>2</v>
@@ -2926,7 +2935,7 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="22"/>
       <c r="C8" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D8" s="24" t="n">
         <v>3</v>
@@ -2948,10 +2957,10 @@
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D9" s="24" t="n">
         <v>1</v>
@@ -2974,7 +2983,7 @@
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="22"/>
       <c r="C10" s="26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D10" s="24" t="n">
         <v>2</v>
@@ -2993,7 +3002,7 @@
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22"/>
       <c r="C11" s="26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D11" s="24" t="n">
         <v>3</v>
@@ -3012,7 +3021,7 @@
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="22"/>
       <c r="C12" s="26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D12" s="24" t="n">
         <v>4</v>
@@ -3030,10 +3039,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D13" s="24" t="n">
         <v>1</v>
@@ -3052,7 +3061,7 @@
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22"/>
       <c r="C14" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D14" s="24" t="n">
         <v>2</v>
@@ -3071,7 +3080,7 @@
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22"/>
       <c r="C15" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D15" s="24" t="n">
         <v>3</v>
@@ -3089,10 +3098,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D16" s="24" t="n">
         <v>1</v>
@@ -3111,7 +3120,7 @@
     <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22"/>
       <c r="C17" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D17" s="24" t="n">
         <v>2</v>
@@ -3130,7 +3139,7 @@
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="22"/>
       <c r="C18" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D18" s="24" t="n">
         <v>3</v>
@@ -3148,10 +3157,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D19" s="24" t="n">
         <v>1</v>
@@ -3170,7 +3179,7 @@
     <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22"/>
       <c r="C20" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D20" s="24" t="n">
         <v>2</v>
@@ -3189,7 +3198,7 @@
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22"/>
       <c r="C21" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D21" s="24" t="n">
         <v>3</v>
@@ -3207,10 +3216,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D22" s="24" t="n">
         <v>1</v>
@@ -3229,7 +3238,7 @@
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22"/>
       <c r="C23" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D23" s="24" t="n">
         <v>2</v>
@@ -3248,7 +3257,7 @@
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22"/>
       <c r="C24" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D24" s="24" t="n">
         <v>3</v>
@@ -3266,10 +3275,10 @@
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D25" s="24" t="n">
         <v>2</v>
@@ -3288,7 +3297,7 @@
     <row r="26" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="22"/>
       <c r="C26" s="26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D26" s="24" t="n">
         <v>3</v>
@@ -3306,10 +3315,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D27" s="24" t="n">
         <v>1</v>
@@ -3328,7 +3337,7 @@
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22"/>
       <c r="C28" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D28" s="24" t="n">
         <v>2</v>
@@ -3347,7 +3356,7 @@
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22"/>
       <c r="C29" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D29" s="24" t="n">
         <v>3</v>
@@ -3365,10 +3374,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D30" s="24" t="n">
         <v>1</v>
@@ -3387,7 +3396,7 @@
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22"/>
       <c r="C31" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D31" s="24" t="n">
         <v>2</v>
@@ -3406,7 +3415,7 @@
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22"/>
       <c r="C32" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D32" s="24" t="n">
         <v>3</v>
@@ -3424,10 +3433,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D33" s="24" t="n">
         <v>1</v>
@@ -3446,7 +3455,7 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22"/>
       <c r="C34" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D34" s="24" t="n">
         <v>2</v>
@@ -3461,7 +3470,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22"/>
       <c r="C35" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D35" s="24" t="n">
         <v>3</v>
@@ -3475,10 +3484,10 @@
     </row>
     <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D36" s="24" t="n">
         <v>2</v>
@@ -3492,10 +3501,10 @@
     </row>
     <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="25" t="n">
@@ -3507,10 +3516,10 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D38" s="24" t="n">
         <v>1</v>
@@ -3525,7 +3534,7 @@
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="22"/>
       <c r="C39" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D39" s="24" t="n">
         <v>2</v>
@@ -3540,7 +3549,7 @@
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="22"/>
       <c r="C40" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D40" s="24" t="n">
         <v>3</v>
@@ -3554,10 +3563,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D41" s="24" t="n">
         <v>1</v>
@@ -3572,7 +3581,7 @@
     <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22"/>
       <c r="C42" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D42" s="24" t="n">
         <v>2</v>
@@ -3587,7 +3596,7 @@
     <row r="43" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22"/>
       <c r="C43" s="26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D43" s="24" t="n">
         <v>3</v>
@@ -3601,10 +3610,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D44" s="24" t="n">
         <v>1</v>
@@ -3619,7 +3628,7 @@
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="22"/>
       <c r="C45" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D45" s="24" t="n">
         <v>2</v>
@@ -3634,7 +3643,7 @@
     <row r="46" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="22"/>
       <c r="C46" s="26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D46" s="24" t="n">
         <v>3</v>
@@ -3648,10 +3657,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D47" s="24" t="n">
         <v>1</v>
@@ -3666,7 +3675,7 @@
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="22"/>
       <c r="C48" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D48" s="24" t="n">
         <v>2</v>
@@ -3681,7 +3690,7 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22"/>
       <c r="C49" s="26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D49" s="24" t="n">
         <v>3</v>
@@ -3695,10 +3704,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="25" t="n">
@@ -3711,7 +3720,7 @@
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22"/>
       <c r="C51" s="26" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D51" s="24"/>
       <c r="E51" s="25" t="n">
@@ -3724,7 +3733,7 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22"/>
       <c r="C52" s="26" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="25" t="n">
@@ -3736,10 +3745,10 @@
     </row>
     <row r="53" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="27" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D53" s="24" t="n">
         <v>1</v>
@@ -3754,7 +3763,7 @@
     <row r="54" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="27"/>
       <c r="C54" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D54" s="24" t="n">
         <v>2</v>
@@ -3769,7 +3778,7 @@
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="27"/>
       <c r="C55" s="26" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D55" s="24" t="n">
         <v>3</v>
@@ -3784,7 +3793,7 @@
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="27"/>
       <c r="C56" s="26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D56" s="24" t="n">
         <v>4</v>
@@ -3798,10 +3807,10 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="27" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C57" s="26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D57" s="24" t="n">
         <v>1</v>
@@ -3816,7 +3825,7 @@
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="27"/>
       <c r="C58" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D58" s="24" t="n">
         <v>2</v>
@@ -3831,7 +3840,7 @@
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="27"/>
       <c r="C59" s="26" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D59" s="24" t="n">
         <v>3</v>
@@ -3846,7 +3855,7 @@
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="27"/>
       <c r="C60" s="26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D60" s="24" t="n">
         <v>4</v>
@@ -3860,10 +3869,10 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="27" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D61" s="24" t="n">
         <v>2</v>
@@ -3878,7 +3887,7 @@
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="27"/>
       <c r="C62" s="26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D62" s="24" t="n">
         <v>3</v>
@@ -3893,7 +3902,7 @@
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="27"/>
       <c r="C63" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D63" s="24" t="n">
         <v>4</v>
@@ -3907,10 +3916,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D64" s="24" t="n">
         <v>2</v>
@@ -3925,10 +3934,10 @@
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="27"/>
       <c r="C65" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E65" s="28" t="n">
         <v>150</v>
@@ -3939,10 +3948,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="27" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D66" s="24" t="n">
         <v>2</v>
@@ -3957,10 +3966,10 @@
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="27"/>
       <c r="C67" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D67" s="24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E67" s="28" t="n">
         <v>72.5</v>
@@ -4043,7 +4052,7 @@
     </row>
     <row r="2" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -4051,13 +4060,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D3" s="32"/>
     </row>
@@ -4073,7 +4082,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B5" s="35" t="n">
         <v>1</v>
@@ -4100,7 +4109,7 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34"/>
       <c r="B7" s="37" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C7" s="38" t="n">
         <v>25.1301775147929</v>
@@ -4111,7 +4120,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B8" s="35" t="n">
         <v>1</v>
@@ -4138,7 +4147,7 @@
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34"/>
       <c r="B10" s="37" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C10" s="38" t="n">
         <v>20.1041420118343</v>
@@ -4149,7 +4158,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B11" s="41" t="n">
         <v>1</v>
@@ -4163,7 +4172,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="43" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B12" s="44" t="n">
         <v>2</v>
@@ -4177,10 +4186,10 @@
     </row>
     <row r="13" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="46" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C13" s="48" t="n">
         <v>20</v>
@@ -4191,12 +4200,12 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4225,7 +4234,7 @@
   </sheetPr>
   <dimension ref="A2:F117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -4242,42 +4251,42 @@
   <sheetData>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="53" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D2" s="54"/>
     </row>
     <row r="3" s="59" customFormat="true" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="55" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="60" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B4" s="27" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E4" s="63" t="n">
         <v>1</v>
@@ -4289,7 +4298,7 @@
       <c r="B5" s="27"/>
       <c r="C5" s="61"/>
       <c r="D5" s="62" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E5" s="63" t="n">
         <v>1</v>
@@ -4301,7 +4310,7 @@
       <c r="B6" s="27"/>
       <c r="C6" s="61"/>
       <c r="D6" s="62" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E6" s="63" t="n">
         <v>1</v>
@@ -4313,7 +4322,7 @@
       <c r="B7" s="27"/>
       <c r="C7" s="61"/>
       <c r="D7" s="62" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E7" s="63" t="n">
         <v>2</v>
@@ -4326,10 +4335,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E8" s="63" t="n">
         <v>1</v>
@@ -4342,10 +4351,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E9" s="63" t="n">
         <v>1</v>
@@ -4357,7 +4366,7 @@
       <c r="B10" s="24"/>
       <c r="C10" s="61"/>
       <c r="D10" s="26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E10" s="63" t="n">
         <v>1</v>
@@ -4369,7 +4378,7 @@
       <c r="B11" s="24"/>
       <c r="C11" s="61"/>
       <c r="D11" s="26" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E11" s="63" t="n">
         <v>1</v>
@@ -4381,7 +4390,7 @@
       <c r="B12" s="24"/>
       <c r="C12" s="61"/>
       <c r="D12" s="26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E12" s="63" t="n">
         <v>1</v>
@@ -4393,7 +4402,7 @@
       <c r="B13" s="24"/>
       <c r="C13" s="61"/>
       <c r="D13" s="26" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E13" s="63" t="n">
         <v>1</v>
@@ -4406,10 +4415,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E14" s="63" t="n">
         <v>2</v>
@@ -4422,10 +4431,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E15" s="22" t="n">
         <v>1</v>
@@ -4438,10 +4447,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E16" s="22" t="n">
         <v>1</v>
@@ -4453,7 +4462,7 @@
       <c r="B17" s="27"/>
       <c r="C17" s="22"/>
       <c r="D17" s="61" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E17" s="22" t="n">
         <v>1</v>
@@ -4465,7 +4474,7 @@
       <c r="B18" s="27"/>
       <c r="C18" s="22"/>
       <c r="D18" s="61" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E18" s="22" t="n">
         <v>1</v>
@@ -4474,16 +4483,16 @@
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="60" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B19" s="24" t="n">
         <v>7</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E19" s="22" t="n">
         <v>1</v>
@@ -4496,10 +4505,10 @@
         <v>8</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E20" s="65" t="n">
         <v>1</v>
@@ -4512,10 +4521,10 @@
         <v>9</v>
       </c>
       <c r="C21" s="61" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E21" s="22" t="n">
         <v>4</v>
@@ -4528,10 +4537,10 @@
         <v>10</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E22" s="65" t="n">
         <v>1</v>
@@ -4544,10 +4553,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E23" s="65" t="n">
         <v>1</v>
@@ -4560,10 +4569,10 @@
         <v>12</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D24" s="61" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E24" s="65" t="n">
         <v>1</v>
@@ -4575,7 +4584,7 @@
       <c r="B25" s="27"/>
       <c r="C25" s="22"/>
       <c r="D25" s="61" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E25" s="65" t="n">
         <v>1</v>
@@ -4584,16 +4593,16 @@
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="60" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B26" s="24" t="n">
         <v>13</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E26" s="63"/>
       <c r="F26" s="64"/>
@@ -4603,7 +4612,7 @@
       <c r="B27" s="24"/>
       <c r="C27" s="22"/>
       <c r="D27" s="61" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E27" s="65" t="n">
         <v>1</v>
@@ -4615,7 +4624,7 @@
       <c r="B28" s="24"/>
       <c r="C28" s="22"/>
       <c r="D28" s="26" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E28" s="65" t="n">
         <v>1</v>
@@ -4627,7 +4636,7 @@
       <c r="B29" s="24"/>
       <c r="C29" s="22"/>
       <c r="D29" s="26" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E29" s="65" t="n">
         <v>1</v>
@@ -4639,7 +4648,7 @@
       <c r="B30" s="24"/>
       <c r="C30" s="22"/>
       <c r="D30" s="26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E30" s="65" t="n">
         <v>1</v>
@@ -4651,7 +4660,7 @@
       <c r="B31" s="24"/>
       <c r="C31" s="22"/>
       <c r="D31" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E31" s="65" t="n">
         <v>1</v>
@@ -4663,7 +4672,7 @@
       <c r="B32" s="24"/>
       <c r="C32" s="22"/>
       <c r="D32" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E32" s="65" t="n">
         <v>1</v>
@@ -4676,10 +4685,10 @@
         <v>14</v>
       </c>
       <c r="C33" s="61" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E33" s="65" t="n">
         <v>1</v>
@@ -4692,10 +4701,10 @@
         <v>15</v>
       </c>
       <c r="C34" s="61" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E34" s="65" t="n">
         <v>1</v>
@@ -4708,10 +4717,10 @@
         <v>16</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E35" s="65" t="n">
         <v>2</v>
@@ -4723,7 +4732,7 @@
       <c r="B36" s="27"/>
       <c r="C36" s="22"/>
       <c r="D36" s="26" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E36" s="65" t="n">
         <v>2</v>
@@ -4736,10 +4745,10 @@
         <v>17</v>
       </c>
       <c r="C37" s="61" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E37" s="65" t="n">
         <v>4</v>
@@ -4748,16 +4757,16 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="60" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B38" s="27" t="n">
         <v>18</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E38" s="63"/>
       <c r="F38" s="64"/>
@@ -4767,7 +4776,7 @@
       <c r="B39" s="27"/>
       <c r="C39" s="22"/>
       <c r="D39" s="26" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E39" s="65" t="n">
         <v>1</v>
@@ -4779,7 +4788,7 @@
       <c r="B40" s="27"/>
       <c r="C40" s="22"/>
       <c r="D40" s="26" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E40" s="65" t="n">
         <v>1</v>
@@ -4792,10 +4801,10 @@
         <v>19</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E41" s="65" t="n">
         <v>1</v>
@@ -4807,7 +4816,7 @@
       <c r="B42" s="27"/>
       <c r="C42" s="22"/>
       <c r="D42" s="26" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E42" s="65" t="n">
         <v>1</v>
@@ -4820,10 +4829,10 @@
         <v>20</v>
       </c>
       <c r="C43" s="61" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E43" s="65" t="n">
         <v>1</v>
@@ -4836,10 +4845,10 @@
         <v>21</v>
       </c>
       <c r="C44" s="61" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E44" s="65" t="n">
         <v>1</v>
@@ -4848,16 +4857,16 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="60" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B45" s="24" t="n">
         <v>22</v>
       </c>
       <c r="C45" s="61" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E45" s="63" t="n">
         <v>1</v>
@@ -4870,10 +4879,10 @@
         <v>23</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E46" s="65" t="n">
         <v>2</v>
@@ -4885,7 +4894,7 @@
       <c r="B47" s="27"/>
       <c r="C47" s="22"/>
       <c r="D47" s="26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E47" s="65" t="n">
         <v>2</v>
@@ -4897,7 +4906,7 @@
       <c r="B48" s="27"/>
       <c r="C48" s="22"/>
       <c r="D48" s="26" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E48" s="65" t="n">
         <v>1</v>
@@ -4910,7 +4919,7 @@
         <v>24</v>
       </c>
       <c r="C49" s="61" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D49" s="26"/>
       <c r="E49" s="65" t="n">
@@ -4924,10 +4933,10 @@
         <v>25</v>
       </c>
       <c r="C50" s="61" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D50" s="61" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E50" s="65" t="n">
         <v>1</v>
@@ -4940,10 +4949,10 @@
         <v>26</v>
       </c>
       <c r="C51" s="61" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D51" s="61" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E51" s="65" t="n">
         <v>2</v>
@@ -4956,7 +4965,7 @@
         <v>27</v>
       </c>
       <c r="C52" s="61" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D52" s="26"/>
       <c r="E52" s="65" t="n">
@@ -4970,10 +4979,10 @@
         <v>28</v>
       </c>
       <c r="C53" s="61" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E53" s="65" t="n">
         <v>4</v>
@@ -4986,7 +4995,7 @@
         <v>29</v>
       </c>
       <c r="C54" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="65" t="n">
@@ -5000,10 +5009,10 @@
         <v>30</v>
       </c>
       <c r="C55" s="61" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D55" s="61" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E55" s="65" t="n">
         <v>1</v>
@@ -5016,10 +5025,10 @@
         <v>31</v>
       </c>
       <c r="C56" s="61" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D56" s="61" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E56" s="65" t="n">
         <v>2</v>
@@ -5032,7 +5041,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="61" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="65" t="n">
@@ -5046,10 +5055,10 @@
         <v>33</v>
       </c>
       <c r="C58" s="61" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D58" s="61" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E58" s="65" t="n">
         <v>2</v>
@@ -5058,16 +5067,16 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="60" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B59" s="24" t="n">
         <v>34</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D59" s="61" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E59" s="65"/>
       <c r="F59" s="64"/>
@@ -5077,7 +5086,7 @@
       <c r="B60" s="24"/>
       <c r="C60" s="22"/>
       <c r="D60" s="61" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E60" s="65" t="n">
         <v>1</v>
@@ -5089,7 +5098,7 @@
       <c r="B61" s="24"/>
       <c r="C61" s="22"/>
       <c r="D61" s="61" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E61" s="65" t="n">
         <v>1</v>
@@ -5101,7 +5110,7 @@
       <c r="B62" s="24"/>
       <c r="C62" s="22"/>
       <c r="D62" s="61" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E62" s="65" t="n">
         <v>1</v>
@@ -5113,7 +5122,7 @@
       <c r="B63" s="24"/>
       <c r="C63" s="22"/>
       <c r="D63" s="61" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E63" s="65" t="n">
         <v>1</v>
@@ -5126,10 +5135,10 @@
         <v>35</v>
       </c>
       <c r="C64" s="61" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D64" s="61" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E64" s="65" t="n">
         <v>2</v>
@@ -5142,10 +5151,10 @@
         <v>36</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D65" s="61" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E65" s="63"/>
       <c r="F65" s="64"/>
@@ -5155,7 +5164,7 @@
       <c r="B66" s="27"/>
       <c r="C66" s="22"/>
       <c r="D66" s="61" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E66" s="65" t="n">
         <v>1</v>
@@ -5167,7 +5176,7 @@
       <c r="B67" s="27"/>
       <c r="C67" s="22"/>
       <c r="D67" s="61" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E67" s="65" t="n">
         <v>1</v>
@@ -5180,10 +5189,10 @@
         <v>37</v>
       </c>
       <c r="C68" s="61" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D68" s="61" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E68" s="65" t="n">
         <v>1</v>
@@ -5192,16 +5201,16 @@
     </row>
     <row r="69" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="60" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B69" s="24" t="n">
         <v>38</v>
       </c>
       <c r="C69" s="61" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D69" s="61" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E69" s="65" t="n">
         <v>1</v>
@@ -5214,10 +5223,10 @@
         <v>39</v>
       </c>
       <c r="C70" s="61" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E70" s="65" t="n">
         <v>2</v>
@@ -5230,10 +5239,10 @@
         <v>40</v>
       </c>
       <c r="C71" s="61" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D71" s="61" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E71" s="65" t="n">
         <v>2</v>
@@ -5246,10 +5255,10 @@
         <v>41</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D72" s="61" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E72" s="65" t="n">
         <v>1</v>
@@ -5261,7 +5270,7 @@
       <c r="B73" s="24"/>
       <c r="C73" s="22"/>
       <c r="D73" s="61" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E73" s="65" t="n">
         <v>1</v>
@@ -5273,7 +5282,7 @@
       <c r="B74" s="24"/>
       <c r="C74" s="22"/>
       <c r="D74" s="61" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E74" s="65" t="n">
         <v>1</v>
@@ -5285,7 +5294,7 @@
       <c r="B75" s="24"/>
       <c r="C75" s="22"/>
       <c r="D75" s="61" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E75" s="65" t="n">
         <v>1</v>
@@ -5297,7 +5306,7 @@
       <c r="B76" s="24"/>
       <c r="C76" s="22"/>
       <c r="D76" s="61" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E76" s="65" t="n">
         <v>1</v>
@@ -5309,7 +5318,7 @@
       <c r="B77" s="24"/>
       <c r="C77" s="22"/>
       <c r="D77" s="61" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E77" s="65" t="n">
         <v>1</v>
@@ -5322,10 +5331,10 @@
         <v>42</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E78" s="65" t="n">
         <v>1</v>
@@ -5337,7 +5346,7 @@
       <c r="B79" s="24"/>
       <c r="C79" s="22"/>
       <c r="D79" s="26" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E79" s="65" t="n">
         <v>1</v>
@@ -5349,7 +5358,7 @@
       <c r="B80" s="24"/>
       <c r="C80" s="22"/>
       <c r="D80" s="26" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E80" s="65" t="n">
         <v>1</v>
@@ -5361,7 +5370,7 @@
       <c r="B81" s="24"/>
       <c r="C81" s="22"/>
       <c r="D81" s="26" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E81" s="65" t="n">
         <v>1</v>
@@ -5373,7 +5382,7 @@
       <c r="B82" s="24"/>
       <c r="C82" s="22"/>
       <c r="D82" s="26" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E82" s="65" t="n">
         <v>1</v>
@@ -5385,7 +5394,7 @@
       <c r="B83" s="24"/>
       <c r="C83" s="22"/>
       <c r="D83" s="26" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E83" s="65" t="n">
         <v>1</v>
@@ -5398,10 +5407,10 @@
         <v>43</v>
       </c>
       <c r="C84" s="61" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E84" s="65" t="n">
         <v>2</v>
@@ -5414,7 +5423,7 @@
         <v>44</v>
       </c>
       <c r="C85" s="61" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D85" s="26"/>
       <c r="E85" s="65" t="n">
@@ -5424,13 +5433,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="60" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B86" s="24" t="n">
         <v>45</v>
       </c>
       <c r="C86" s="61" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D86" s="26"/>
       <c r="E86" s="65" t="n">
@@ -5444,7 +5453,7 @@
         <v>46</v>
       </c>
       <c r="C87" s="61" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D87" s="26"/>
       <c r="E87" s="65" t="n">
@@ -5458,7 +5467,7 @@
         <v>47</v>
       </c>
       <c r="C88" s="61" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D88" s="26"/>
       <c r="E88" s="65" t="n">
@@ -5472,10 +5481,10 @@
         <v>48</v>
       </c>
       <c r="C89" s="61" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E89" s="65" t="n">
         <v>1</v>
@@ -5488,7 +5497,7 @@
         <v>49</v>
       </c>
       <c r="C90" s="61" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D90" s="26"/>
       <c r="E90" s="65" t="n">
@@ -5502,10 +5511,10 @@
         <v>50</v>
       </c>
       <c r="C91" s="61" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E91" s="65" t="n">
         <v>2</v>
@@ -5514,16 +5523,16 @@
     </row>
     <row r="92" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="60" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B92" s="24" t="n">
         <v>51</v>
       </c>
       <c r="C92" s="61" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E92" s="63" t="n">
         <v>4</v>
@@ -5536,10 +5545,10 @@
         <v>52</v>
       </c>
       <c r="C93" s="61" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E93" s="63" t="n">
         <v>1</v>
@@ -5552,7 +5561,7 @@
         <v>53</v>
       </c>
       <c r="C94" s="61" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D94" s="26"/>
       <c r="E94" s="63" t="n">
@@ -5566,7 +5575,7 @@
         <v>54</v>
       </c>
       <c r="C95" s="61" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D95" s="26"/>
       <c r="E95" s="63" t="n">
@@ -5580,10 +5589,10 @@
         <v>55</v>
       </c>
       <c r="C96" s="61" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E96" s="63" t="n">
         <v>1</v>
@@ -5596,10 +5605,10 @@
         <v>56</v>
       </c>
       <c r="C97" s="61" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E97" s="63" t="n">
         <v>1</v>
@@ -5612,10 +5621,10 @@
         <v>57</v>
       </c>
       <c r="C98" s="61" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E98" s="63" t="n">
         <v>1</v>
@@ -5628,10 +5637,10 @@
         <v>58</v>
       </c>
       <c r="C99" s="61" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E99" s="63" t="n">
         <v>1</v>
@@ -5644,7 +5653,7 @@
         <v>59</v>
       </c>
       <c r="C100" s="61" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D100" s="26"/>
       <c r="E100" s="63" t="n">
@@ -5658,7 +5667,7 @@
         <v>60</v>
       </c>
       <c r="C101" s="61" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D101" s="26"/>
       <c r="E101" s="63" t="n">
@@ -5672,10 +5681,10 @@
         <v>61</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E102" s="63" t="n">
         <v>1</v>
@@ -5687,7 +5696,7 @@
       <c r="B103" s="27"/>
       <c r="C103" s="22"/>
       <c r="D103" s="26" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E103" s="63" t="n">
         <v>1</v>
@@ -5699,7 +5708,7 @@
       <c r="B104" s="27"/>
       <c r="C104" s="22"/>
       <c r="D104" s="26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E104" s="63" t="n">
         <v>1</v>
@@ -5711,7 +5720,7 @@
       <c r="B105" s="27"/>
       <c r="C105" s="22"/>
       <c r="D105" s="26" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E105" s="63" t="n">
         <v>1</v>
@@ -5724,10 +5733,10 @@
         <v>62</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E106" s="63" t="n">
         <v>1</v>
@@ -5739,7 +5748,7 @@
       <c r="B107" s="24"/>
       <c r="C107" s="22"/>
       <c r="D107" s="26" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E107" s="63" t="n">
         <v>1</v>
@@ -5751,7 +5760,7 @@
       <c r="B108" s="24"/>
       <c r="C108" s="22"/>
       <c r="D108" s="26" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E108" s="63" t="n">
         <v>1</v>
@@ -5763,7 +5772,7 @@
       <c r="B109" s="24"/>
       <c r="C109" s="22"/>
       <c r="D109" s="26" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E109" s="63" t="n">
         <v>1</v>
@@ -5775,7 +5784,7 @@
       <c r="B110" s="24"/>
       <c r="C110" s="22"/>
       <c r="D110" s="26" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E110" s="63" t="n">
         <v>1</v>
@@ -5787,7 +5796,7 @@
       <c r="B111" s="24"/>
       <c r="C111" s="22"/>
       <c r="D111" s="26" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E111" s="63" t="n">
         <v>1</v>
@@ -5800,7 +5809,7 @@
         <v>63</v>
       </c>
       <c r="C112" s="61" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D112" s="26"/>
       <c r="E112" s="63" t="n">
@@ -5814,7 +5823,7 @@
         <v>64</v>
       </c>
       <c r="C113" s="61" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D113" s="26"/>
       <c r="E113" s="63" t="n">
@@ -5828,7 +5837,7 @@
         <v>65</v>
       </c>
       <c r="C114" s="61" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D114" s="26"/>
       <c r="E114" s="63" t="n">
@@ -5842,7 +5851,7 @@
         <v>66</v>
       </c>
       <c r="C115" s="61" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D115" s="26"/>
       <c r="E115" s="63" t="n">
@@ -5856,7 +5865,7 @@
         <v>67</v>
       </c>
       <c r="C116" s="61" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D116" s="26"/>
       <c r="E116" s="63" t="n">
@@ -5870,7 +5879,7 @@
         <v>68</v>
       </c>
       <c r="C117" s="61" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D117" s="26"/>
       <c r="E117" s="63" t="n">
@@ -5953,54 +5962,54 @@
   <sheetData>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="67" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C2" s="67"/>
       <c r="D2" s="67"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="68" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="71" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B4" s="24" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D4" s="72" t="n">
         <v>0.2</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="73" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B5" s="74" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D5" s="72" t="n">
         <v>0.2</v>
@@ -6013,7 +6022,7 @@
       <c r="A6" s="73"/>
       <c r="B6" s="74"/>
       <c r="C6" s="75" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D6" s="77" t="n">
         <v>0.15</v>
@@ -6024,13 +6033,13 @@
     </row>
     <row r="7" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="78" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B7" s="74" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D7" s="77" t="n">
         <v>0.3</v>
@@ -6043,7 +6052,7 @@
       <c r="A8" s="78"/>
       <c r="B8" s="74"/>
       <c r="C8" s="79" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D8" s="77" t="n">
         <v>0.15</v>
@@ -6056,7 +6065,7 @@
       <c r="A9" s="78"/>
       <c r="B9" s="74"/>
       <c r="C9" s="79" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D9" s="77" t="n">
         <v>0.15</v>
@@ -6067,13 +6076,13 @@
     </row>
     <row r="10" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="78" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B10" s="74" t="n">
         <v>4</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D10" s="77" t="n">
         <v>-0.3</v>
@@ -6086,7 +6095,7 @@
       <c r="A11" s="78"/>
       <c r="B11" s="74"/>
       <c r="C11" s="79" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D11" s="77" t="n">
         <v>-0.3</v>
@@ -6097,13 +6106,13 @@
     </row>
     <row r="12" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="78" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B12" s="74" t="n">
         <v>5</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D12" s="77" t="n">
         <v>0.3</v>
@@ -6116,7 +6125,7 @@
       <c r="A13" s="78"/>
       <c r="B13" s="74"/>
       <c r="C13" s="79" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D13" s="77" t="n">
         <v>0.4</v>
@@ -6129,7 +6138,7 @@
       <c r="A14" s="78"/>
       <c r="B14" s="74"/>
       <c r="C14" s="79" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D14" s="77" t="n">
         <v>0.4</v>
@@ -6183,7 +6192,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="69.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="83" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6191,99 +6200,99 @@
     </row>
     <row r="4" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="84" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C4" s="84" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D4" s="85" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="84" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="85" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="84"/>
       <c r="C6" s="84"/>
       <c r="D6" s="85" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="84"/>
       <c r="C7" s="84"/>
       <c r="D7" s="85" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="84"/>
       <c r="C8" s="84"/>
       <c r="D8" s="85" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="84"/>
       <c r="C9" s="84"/>
       <c r="D9" s="85" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="84"/>
       <c r="C10" s="84"/>
       <c r="D10" s="85" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="84" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C11" s="84" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D11" s="85" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="84" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C12" s="84" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D12" s="85" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="84" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C13" s="85" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D13" s="85" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="84" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C14" s="84"/>
       <c r="D14" s="86" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E14" s="87"/>
       <c r="F14" s="88"/>
@@ -6291,10 +6300,10 @@
     <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="89"/>
       <c r="C15" s="90" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#127 model Order cheged....
</commit_message>
<xml_diff>
--- a/VOKSS прейскурант_ 2.xlsx
+++ b/VOKSS прейскурант_ 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="розподіл матеріалів (Fabric)" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="406">
   <si>
     <t xml:space="preserve">Примерное распределение материалов по группам сложности в зависимости от трудоѐмкости обработки</t>
   </si>
@@ -582,6 +582,12 @@
   </si>
   <si>
     <t xml:space="preserve">ПЕРЕЧЕНЬ усложняющих элементов (сверх количества, учтѐнного в минимальной сложности)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">додати можливість вибору!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">умовна одиниця</t>
   </si>
   <si>
     <t xml:space="preserve">Групи елементів</t>
@@ -1375,7 +1381,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1398,6 +1404,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE5CA"/>
         <bgColor rgb="FFE0EFD4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED1C24"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -1610,7 +1622,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1829,6 +1841,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2012,7 +2032,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
@@ -2078,7 +2098,7 @@
   </sheetPr>
   <dimension ref="B2:D35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2295,7 +2315,7 @@
   </sheetPr>
   <dimension ref="B1:B78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
     </sheetView>
   </sheetViews>
@@ -3947,7 +3967,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4147,7 +4167,7 @@
   <dimension ref="A2:F117"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4166,1644 +4186,1650 @@
         <v>178</v>
       </c>
       <c r="D2" s="54"/>
-    </row>
-    <row r="3" s="59" customFormat="true" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="55" t="s">
+      <c r="E2" s="55" t="s">
         <v>179</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="F2" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="C3" s="57" t="s">
+    </row>
+    <row r="3" s="61" customFormat="true" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="B3" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="C3" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="D3" s="59" t="s">
         <v>184</v>
       </c>
+      <c r="E3" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="60" t="s">
-        <v>185</v>
+      <c r="A4" s="62" t="s">
+        <v>187</v>
       </c>
       <c r="B4" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>187</v>
-      </c>
-      <c r="E4" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="64" t="s">
+      <c r="C4" s="63" t="s">
         <v>188</v>
       </c>
+      <c r="D4" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="66" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="60"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="27"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62" t="s">
-        <v>189</v>
-      </c>
-      <c r="E5" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="64" t="s">
-        <v>190</v>
+      <c r="C5" s="63"/>
+      <c r="D5" s="64" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="66" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="27"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="62" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="64" t="s">
-        <v>192</v>
+      <c r="C6" s="63"/>
+      <c r="D6" s="64" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="60"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="E7" s="63" t="n">
+      <c r="C7" s="63"/>
+      <c r="D7" s="64" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="65" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="64"/>
+      <c r="F7" s="66"/>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="60"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="61" t="s">
-        <v>194</v>
+      <c r="C8" s="63" t="s">
+        <v>196</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="E8" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="64"/>
+        <v>197</v>
+      </c>
+      <c r="E8" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="66"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="60"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="61" t="s">
-        <v>196</v>
+      <c r="C9" s="63" t="s">
+        <v>198</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="64"/>
+        <v>199</v>
+      </c>
+      <c r="E9" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="66"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="60"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="24"/>
-      <c r="C10" s="61"/>
+      <c r="C10" s="63"/>
       <c r="D10" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="E10" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="64"/>
+        <v>200</v>
+      </c>
+      <c r="E10" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="66"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="60"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="24"/>
-      <c r="C11" s="61"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="E11" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="64"/>
+        <v>201</v>
+      </c>
+      <c r="E11" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="66"/>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="60"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="24"/>
-      <c r="C12" s="61"/>
+      <c r="C12" s="63"/>
       <c r="D12" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E12" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="64"/>
+        <v>202</v>
+      </c>
+      <c r="E12" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="66"/>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="60"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="24"/>
-      <c r="C13" s="61"/>
+      <c r="C13" s="63"/>
       <c r="D13" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="E13" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="64"/>
+        <v>203</v>
+      </c>
+      <c r="E13" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="66"/>
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="60"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="61" t="s">
-        <v>202</v>
+      <c r="C14" s="63" t="s">
+        <v>204</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="E14" s="63" t="n">
+        <v>205</v>
+      </c>
+      <c r="E14" s="65" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="64"/>
+      <c r="F14" s="66"/>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="60"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="61" t="s">
-        <v>204</v>
-      </c>
-      <c r="D15" s="61" t="s">
-        <v>205</v>
+      <c r="C15" s="63" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>207</v>
       </c>
       <c r="E15" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="64"/>
+      <c r="F15" s="66"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="60"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="27" t="n">
         <v>6</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="D16" s="61" t="s">
-        <v>207</v>
+        <v>208</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>209</v>
       </c>
       <c r="E16" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="64"/>
+      <c r="F16" s="66"/>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="60"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="27"/>
       <c r="C17" s="22"/>
-      <c r="D17" s="61" t="s">
-        <v>208</v>
+      <c r="D17" s="63" t="s">
+        <v>210</v>
       </c>
       <c r="E17" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="64"/>
+      <c r="F17" s="66"/>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="60"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="27"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="61" t="s">
-        <v>209</v>
+      <c r="D18" s="63" t="s">
+        <v>211</v>
       </c>
       <c r="E18" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="64"/>
+      <c r="F18" s="66"/>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="60" t="s">
-        <v>210</v>
+      <c r="A19" s="62" t="s">
+        <v>212</v>
       </c>
       <c r="B19" s="24" t="n">
         <v>7</v>
       </c>
-      <c r="C19" s="61" t="s">
-        <v>211</v>
-      </c>
-      <c r="D19" s="61" t="s">
-        <v>212</v>
+      <c r="C19" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>214</v>
       </c>
       <c r="E19" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="64"/>
+      <c r="F19" s="66"/>
     </row>
     <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="60"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="C20" s="61" t="s">
-        <v>213</v>
-      </c>
-      <c r="D20" s="61" t="s">
-        <v>214</v>
-      </c>
-      <c r="E20" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="64"/>
+      <c r="C20" s="63" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="66"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="60"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="24" t="n">
         <v>9</v>
       </c>
-      <c r="C21" s="61" t="s">
-        <v>215</v>
-      </c>
-      <c r="D21" s="61" t="s">
-        <v>216</v>
+      <c r="C21" s="63" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>218</v>
       </c>
       <c r="E21" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="F21" s="64"/>
+      <c r="F21" s="66"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="60"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="24" t="n">
         <v>10</v>
       </c>
-      <c r="C22" s="61" t="s">
-        <v>217</v>
-      </c>
-      <c r="D22" s="61" t="s">
-        <v>218</v>
-      </c>
-      <c r="E22" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="64"/>
+      <c r="C22" s="63" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>220</v>
+      </c>
+      <c r="E22" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="66"/>
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="60"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="24" t="n">
         <v>11</v>
       </c>
-      <c r="C23" s="61" t="s">
-        <v>219</v>
-      </c>
-      <c r="D23" s="61" t="s">
-        <v>220</v>
-      </c>
-      <c r="E23" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="64"/>
+      <c r="C23" s="63" t="s">
+        <v>221</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>222</v>
+      </c>
+      <c r="E23" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="66"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="60"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="27" t="n">
         <v>12</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="D24" s="61" t="s">
-        <v>222</v>
-      </c>
-      <c r="E24" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F24" s="64"/>
+        <v>223</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="66"/>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="60"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="27"/>
       <c r="C25" s="22"/>
-      <c r="D25" s="61" t="s">
-        <v>223</v>
-      </c>
-      <c r="E25" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" s="64"/>
+      <c r="D25" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E25" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="66"/>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="60" t="s">
-        <v>224</v>
+      <c r="A26" s="62" t="s">
+        <v>226</v>
       </c>
       <c r="B26" s="24" t="n">
         <v>13</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="D26" s="61" t="s">
-        <v>226</v>
-      </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="64"/>
+        <v>227</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>228</v>
+      </c>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="60"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="24"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="61" t="s">
-        <v>227</v>
-      </c>
-      <c r="E27" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" s="64"/>
+      <c r="D27" s="63" t="s">
+        <v>229</v>
+      </c>
+      <c r="E27" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="66"/>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="60"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="24"/>
       <c r="C28" s="22"/>
       <c r="D28" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="E28" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" s="64"/>
+        <v>230</v>
+      </c>
+      <c r="E28" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="66"/>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="60"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="24"/>
       <c r="C29" s="22"/>
       <c r="D29" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E29" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F29" s="64"/>
+        <v>231</v>
+      </c>
+      <c r="E29" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="66"/>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="60"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="24"/>
       <c r="C30" s="22"/>
       <c r="D30" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="E30" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" s="64"/>
+        <v>232</v>
+      </c>
+      <c r="E30" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="66"/>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="60"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="24"/>
       <c r="C31" s="22"/>
       <c r="D31" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="E31" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" s="64"/>
+        <v>233</v>
+      </c>
+      <c r="E31" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="66"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="60"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="24"/>
       <c r="C32" s="22"/>
       <c r="D32" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="E32" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" s="64"/>
+        <v>234</v>
+      </c>
+      <c r="E32" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" s="66"/>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="60"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="24" t="n">
         <v>14</v>
       </c>
-      <c r="C33" s="61" t="s">
-        <v>233</v>
+      <c r="C33" s="63" t="s">
+        <v>235</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="E33" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" s="64"/>
+        <v>236</v>
+      </c>
+      <c r="E33" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="66"/>
     </row>
     <row r="34" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="60"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="24" t="n">
         <v>15</v>
       </c>
-      <c r="C34" s="61" t="s">
-        <v>235</v>
+      <c r="C34" s="63" t="s">
+        <v>237</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="E34" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="64"/>
+        <v>238</v>
+      </c>
+      <c r="E34" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="66"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="60"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="27" t="n">
         <v>16</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="E35" s="65" t="n">
+        <v>240</v>
+      </c>
+      <c r="E35" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F35" s="64"/>
+      <c r="F35" s="66"/>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="60"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="27"/>
       <c r="C36" s="22"/>
       <c r="D36" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="E36" s="65" t="n">
+        <v>241</v>
+      </c>
+      <c r="E36" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F36" s="64"/>
+      <c r="F36" s="66"/>
     </row>
     <row r="37" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="60"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="24" t="n">
         <v>17</v>
       </c>
-      <c r="C37" s="61" t="s">
-        <v>240</v>
+      <c r="C37" s="63" t="s">
+        <v>242</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="E37" s="65" t="n">
+        <v>243</v>
+      </c>
+      <c r="E37" s="67" t="n">
         <v>4</v>
       </c>
-      <c r="F37" s="64"/>
+      <c r="F37" s="66"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="60" t="s">
-        <v>242</v>
+      <c r="A38" s="62" t="s">
+        <v>244</v>
       </c>
       <c r="B38" s="27" t="n">
         <v>18</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="64"/>
+        <v>246</v>
+      </c>
+      <c r="E38" s="65"/>
+      <c r="F38" s="66"/>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="60"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="27"/>
       <c r="C39" s="22"/>
       <c r="D39" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="E39" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" s="64"/>
+        <v>247</v>
+      </c>
+      <c r="E39" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="66"/>
     </row>
     <row r="40" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="60"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="27"/>
       <c r="C40" s="22"/>
       <c r="D40" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="E40" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F40" s="64"/>
+        <v>248</v>
+      </c>
+      <c r="E40" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="66"/>
     </row>
     <row r="41" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="60"/>
+      <c r="A41" s="62"/>
       <c r="B41" s="27" t="n">
         <v>19</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="E41" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="64"/>
+        <v>250</v>
+      </c>
+      <c r="E41" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="66"/>
     </row>
     <row r="42" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="60"/>
+      <c r="A42" s="62"/>
       <c r="B42" s="27"/>
       <c r="C42" s="22"/>
       <c r="D42" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="E42" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" s="64"/>
+        <v>251</v>
+      </c>
+      <c r="E42" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="66"/>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="60"/>
+      <c r="A43" s="62"/>
       <c r="B43" s="24" t="n">
         <v>20</v>
       </c>
-      <c r="C43" s="61" t="s">
-        <v>250</v>
+      <c r="C43" s="63" t="s">
+        <v>252</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="E43" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" s="64"/>
+        <v>253</v>
+      </c>
+      <c r="E43" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="66"/>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="60"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="24" t="n">
         <v>21</v>
       </c>
-      <c r="C44" s="61" t="s">
-        <v>252</v>
+      <c r="C44" s="63" t="s">
+        <v>254</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E44" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" s="64"/>
+        <v>255</v>
+      </c>
+      <c r="E44" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" s="66"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="60" t="s">
-        <v>254</v>
+      <c r="A45" s="62" t="s">
+        <v>256</v>
       </c>
       <c r="B45" s="24" t="n">
         <v>22</v>
       </c>
-      <c r="C45" s="61" t="s">
-        <v>255</v>
+      <c r="C45" s="63" t="s">
+        <v>257</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>256</v>
-      </c>
-      <c r="E45" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" s="64"/>
+        <v>258</v>
+      </c>
+      <c r="E45" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="66"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="60"/>
+      <c r="A46" s="62"/>
       <c r="B46" s="27" t="n">
         <v>23</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="E46" s="65" t="n">
+        <v>260</v>
+      </c>
+      <c r="E46" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F46" s="64"/>
+      <c r="F46" s="66"/>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="60"/>
+      <c r="A47" s="62"/>
       <c r="B47" s="27"/>
       <c r="C47" s="22"/>
       <c r="D47" s="26" t="s">
-        <v>259</v>
-      </c>
-      <c r="E47" s="65" t="n">
+        <v>261</v>
+      </c>
+      <c r="E47" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F47" s="64"/>
+      <c r="F47" s="66"/>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="60"/>
+      <c r="A48" s="62"/>
       <c r="B48" s="27"/>
       <c r="C48" s="22"/>
       <c r="D48" s="26" t="s">
-        <v>260</v>
-      </c>
-      <c r="E48" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" s="64"/>
+        <v>262</v>
+      </c>
+      <c r="E48" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="66"/>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="60"/>
+      <c r="A49" s="62"/>
       <c r="B49" s="24" t="n">
         <v>24</v>
       </c>
-      <c r="C49" s="61" t="s">
-        <v>261</v>
+      <c r="C49" s="63" t="s">
+        <v>263</v>
       </c>
       <c r="D49" s="26"/>
-      <c r="E49" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" s="64"/>
+      <c r="E49" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="66"/>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="60"/>
+      <c r="A50" s="62"/>
       <c r="B50" s="24" t="n">
         <v>25</v>
       </c>
-      <c r="C50" s="61" t="s">
-        <v>262</v>
-      </c>
-      <c r="D50" s="61" t="s">
-        <v>263</v>
-      </c>
-      <c r="E50" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" s="64"/>
+      <c r="C50" s="63" t="s">
+        <v>264</v>
+      </c>
+      <c r="D50" s="63" t="s">
+        <v>265</v>
+      </c>
+      <c r="E50" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="66"/>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="60"/>
+      <c r="A51" s="62"/>
       <c r="B51" s="24" t="n">
         <v>26</v>
       </c>
-      <c r="C51" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D51" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="E51" s="65" t="n">
+      <c r="C51" s="63" t="s">
+        <v>266</v>
+      </c>
+      <c r="D51" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="E51" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F51" s="64"/>
+      <c r="F51" s="66"/>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="60"/>
+      <c r="A52" s="62"/>
       <c r="B52" s="24" t="n">
         <v>27</v>
       </c>
-      <c r="C52" s="61" t="s">
-        <v>266</v>
+      <c r="C52" s="63" t="s">
+        <v>268</v>
       </c>
       <c r="D52" s="26"/>
-      <c r="E52" s="65" t="n">
+      <c r="E52" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F52" s="64"/>
+      <c r="F52" s="66"/>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="60"/>
+      <c r="A53" s="62"/>
       <c r="B53" s="24" t="n">
         <v>28</v>
       </c>
-      <c r="C53" s="61" t="s">
+      <c r="C53" s="63" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="D53" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="E53" s="65" t="n">
+      <c r="E53" s="67" t="n">
         <v>4</v>
       </c>
-      <c r="F53" s="64"/>
+      <c r="F53" s="66"/>
     </row>
     <row r="54" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="60"/>
+      <c r="A54" s="62"/>
       <c r="B54" s="24" t="n">
         <v>29</v>
       </c>
-      <c r="C54" s="61" t="s">
-        <v>268</v>
+      <c r="C54" s="63" t="s">
+        <v>270</v>
       </c>
       <c r="D54" s="26"/>
-      <c r="E54" s="65" t="n">
+      <c r="E54" s="67" t="n">
         <v>4</v>
       </c>
-      <c r="F54" s="64"/>
+      <c r="F54" s="66"/>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="60"/>
+      <c r="A55" s="62"/>
       <c r="B55" s="24" t="n">
         <v>30</v>
       </c>
-      <c r="C55" s="61" t="s">
-        <v>269</v>
-      </c>
-      <c r="D55" s="61" t="s">
-        <v>270</v>
-      </c>
-      <c r="E55" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F55" s="64"/>
+      <c r="C55" s="63" t="s">
+        <v>271</v>
+      </c>
+      <c r="D55" s="63" t="s">
+        <v>272</v>
+      </c>
+      <c r="E55" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" s="66"/>
     </row>
     <row r="56" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="60"/>
+      <c r="A56" s="62"/>
       <c r="B56" s="24" t="n">
         <v>31</v>
       </c>
-      <c r="C56" s="61" t="s">
-        <v>271</v>
-      </c>
-      <c r="D56" s="61" t="s">
-        <v>272</v>
-      </c>
-      <c r="E56" s="65" t="n">
+      <c r="C56" s="63" t="s">
+        <v>273</v>
+      </c>
+      <c r="D56" s="63" t="s">
+        <v>274</v>
+      </c>
+      <c r="E56" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F56" s="64"/>
+      <c r="F56" s="66"/>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="60"/>
+      <c r="A57" s="62"/>
       <c r="B57" s="24" t="n">
         <v>32</v>
       </c>
-      <c r="C57" s="61" t="s">
-        <v>273</v>
+      <c r="C57" s="63" t="s">
+        <v>275</v>
       </c>
       <c r="D57" s="26"/>
-      <c r="E57" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F57" s="64"/>
+      <c r="E57" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" s="66"/>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="60"/>
+      <c r="A58" s="62"/>
       <c r="B58" s="24" t="n">
         <v>33</v>
       </c>
-      <c r="C58" s="61" t="s">
-        <v>274</v>
-      </c>
-      <c r="D58" s="61" t="s">
-        <v>275</v>
-      </c>
-      <c r="E58" s="65" t="n">
+      <c r="C58" s="63" t="s">
+        <v>276</v>
+      </c>
+      <c r="D58" s="63" t="s">
+        <v>277</v>
+      </c>
+      <c r="E58" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F58" s="64"/>
+      <c r="F58" s="66"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="60" t="s">
-        <v>276</v>
+      <c r="A59" s="62" t="s">
+        <v>278</v>
       </c>
       <c r="B59" s="24" t="n">
         <v>34</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="D59" s="61" t="s">
-        <v>278</v>
-      </c>
-      <c r="E59" s="65"/>
-      <c r="F59" s="64"/>
+        <v>279</v>
+      </c>
+      <c r="D59" s="63" t="s">
+        <v>280</v>
+      </c>
+      <c r="E59" s="67"/>
+      <c r="F59" s="66"/>
     </row>
     <row r="60" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="60"/>
+      <c r="A60" s="62"/>
       <c r="B60" s="24"/>
       <c r="C60" s="22"/>
-      <c r="D60" s="61" t="s">
-        <v>279</v>
-      </c>
-      <c r="E60" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F60" s="64"/>
+      <c r="D60" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="E60" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" s="66"/>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="60"/>
+      <c r="A61" s="62"/>
       <c r="B61" s="24"/>
       <c r="C61" s="22"/>
-      <c r="D61" s="61" t="s">
-        <v>280</v>
-      </c>
-      <c r="E61" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F61" s="64"/>
+      <c r="D61" s="63" t="s">
+        <v>282</v>
+      </c>
+      <c r="E61" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" s="66"/>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="60"/>
+      <c r="A62" s="62"/>
       <c r="B62" s="24"/>
       <c r="C62" s="22"/>
-      <c r="D62" s="61" t="s">
-        <v>281</v>
-      </c>
-      <c r="E62" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" s="64"/>
+      <c r="D62" s="63" t="s">
+        <v>283</v>
+      </c>
+      <c r="E62" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" s="66"/>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="60"/>
+      <c r="A63" s="62"/>
       <c r="B63" s="24"/>
       <c r="C63" s="22"/>
-      <c r="D63" s="61" t="s">
-        <v>282</v>
-      </c>
-      <c r="E63" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F63" s="64"/>
+      <c r="D63" s="63" t="s">
+        <v>284</v>
+      </c>
+      <c r="E63" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="66"/>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="60"/>
+      <c r="A64" s="62"/>
       <c r="B64" s="24" t="n">
         <v>35</v>
       </c>
-      <c r="C64" s="61" t="s">
-        <v>283</v>
-      </c>
-      <c r="D64" s="61" t="s">
-        <v>284</v>
-      </c>
-      <c r="E64" s="65" t="n">
+      <c r="C64" s="63" t="s">
+        <v>285</v>
+      </c>
+      <c r="D64" s="63" t="s">
+        <v>286</v>
+      </c>
+      <c r="E64" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F64" s="64"/>
+      <c r="F64" s="66"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="60"/>
+      <c r="A65" s="62"/>
       <c r="B65" s="27" t="n">
         <v>36</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="D65" s="61" t="s">
-        <v>286</v>
-      </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="64"/>
+        <v>287</v>
+      </c>
+      <c r="D65" s="63" t="s">
+        <v>288</v>
+      </c>
+      <c r="E65" s="65"/>
+      <c r="F65" s="66"/>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="60"/>
+      <c r="A66" s="62"/>
       <c r="B66" s="27"/>
       <c r="C66" s="22"/>
-      <c r="D66" s="61" t="s">
-        <v>287</v>
-      </c>
-      <c r="E66" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" s="64"/>
+      <c r="D66" s="63" t="s">
+        <v>289</v>
+      </c>
+      <c r="E66" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" s="66"/>
     </row>
     <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="60"/>
+      <c r="A67" s="62"/>
       <c r="B67" s="27"/>
       <c r="C67" s="22"/>
-      <c r="D67" s="61" t="s">
-        <v>288</v>
-      </c>
-      <c r="E67" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F67" s="64"/>
+      <c r="D67" s="63" t="s">
+        <v>290</v>
+      </c>
+      <c r="E67" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" s="66"/>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="60"/>
+      <c r="A68" s="62"/>
       <c r="B68" s="24" t="n">
         <v>37</v>
       </c>
-      <c r="C68" s="61" t="s">
-        <v>289</v>
-      </c>
-      <c r="D68" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="E68" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F68" s="64"/>
+      <c r="C68" s="63" t="s">
+        <v>291</v>
+      </c>
+      <c r="D68" s="63" t="s">
+        <v>292</v>
+      </c>
+      <c r="E68" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" s="66"/>
     </row>
     <row r="69" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="60" t="s">
-        <v>291</v>
+      <c r="A69" s="62" t="s">
+        <v>293</v>
       </c>
       <c r="B69" s="24" t="n">
         <v>38</v>
       </c>
-      <c r="C69" s="61" t="s">
-        <v>292</v>
-      </c>
-      <c r="D69" s="61" t="s">
-        <v>293</v>
-      </c>
-      <c r="E69" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F69" s="64"/>
+      <c r="C69" s="63" t="s">
+        <v>294</v>
+      </c>
+      <c r="D69" s="63" t="s">
+        <v>295</v>
+      </c>
+      <c r="E69" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" s="66"/>
     </row>
     <row r="70" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="60"/>
+      <c r="A70" s="62"/>
       <c r="B70" s="24" t="n">
         <v>39</v>
       </c>
-      <c r="C70" s="61" t="s">
-        <v>294</v>
+      <c r="C70" s="63" t="s">
+        <v>296</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="E70" s="65" t="n">
+        <v>297</v>
+      </c>
+      <c r="E70" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F70" s="64"/>
+      <c r="F70" s="66"/>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="60"/>
+      <c r="A71" s="62"/>
       <c r="B71" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="C71" s="61" t="s">
-        <v>296</v>
-      </c>
-      <c r="D71" s="61" t="s">
-        <v>297</v>
-      </c>
-      <c r="E71" s="65" t="n">
+      <c r="C71" s="63" t="s">
+        <v>298</v>
+      </c>
+      <c r="D71" s="63" t="s">
+        <v>299</v>
+      </c>
+      <c r="E71" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F71" s="64"/>
+      <c r="F71" s="66"/>
     </row>
     <row r="72" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="60"/>
+      <c r="A72" s="62"/>
       <c r="B72" s="24" t="n">
         <v>41</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>298</v>
-      </c>
-      <c r="D72" s="61" t="s">
-        <v>299</v>
-      </c>
-      <c r="E72" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F72" s="64"/>
+        <v>300</v>
+      </c>
+      <c r="D72" s="63" t="s">
+        <v>301</v>
+      </c>
+      <c r="E72" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" s="66"/>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="60"/>
+      <c r="A73" s="62"/>
       <c r="B73" s="24"/>
       <c r="C73" s="22"/>
-      <c r="D73" s="61" t="s">
-        <v>300</v>
-      </c>
-      <c r="E73" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F73" s="64"/>
+      <c r="D73" s="63" t="s">
+        <v>302</v>
+      </c>
+      <c r="E73" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" s="66"/>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="60"/>
+      <c r="A74" s="62"/>
       <c r="B74" s="24"/>
       <c r="C74" s="22"/>
-      <c r="D74" s="61" t="s">
-        <v>301</v>
-      </c>
-      <c r="E74" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F74" s="64"/>
+      <c r="D74" s="63" t="s">
+        <v>303</v>
+      </c>
+      <c r="E74" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" s="66"/>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="60"/>
+      <c r="A75" s="62"/>
       <c r="B75" s="24"/>
       <c r="C75" s="22"/>
-      <c r="D75" s="61" t="s">
-        <v>302</v>
-      </c>
-      <c r="E75" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F75" s="64"/>
+      <c r="D75" s="63" t="s">
+        <v>304</v>
+      </c>
+      <c r="E75" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" s="66"/>
     </row>
     <row r="76" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="60"/>
+      <c r="A76" s="62"/>
       <c r="B76" s="24"/>
       <c r="C76" s="22"/>
-      <c r="D76" s="61" t="s">
-        <v>303</v>
-      </c>
-      <c r="E76" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F76" s="64"/>
+      <c r="D76" s="63" t="s">
+        <v>305</v>
+      </c>
+      <c r="E76" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" s="66"/>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="60"/>
+      <c r="A77" s="62"/>
       <c r="B77" s="24"/>
       <c r="C77" s="22"/>
-      <c r="D77" s="61" t="s">
-        <v>304</v>
-      </c>
-      <c r="E77" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F77" s="64"/>
+      <c r="D77" s="63" t="s">
+        <v>306</v>
+      </c>
+      <c r="E77" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" s="66"/>
     </row>
     <row r="78" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="60"/>
+      <c r="A78" s="62"/>
       <c r="B78" s="24" t="n">
         <v>42</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>306</v>
-      </c>
-      <c r="E78" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F78" s="64"/>
+        <v>308</v>
+      </c>
+      <c r="E78" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" s="66"/>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="60"/>
+      <c r="A79" s="62"/>
       <c r="B79" s="24"/>
       <c r="C79" s="22"/>
       <c r="D79" s="26" t="s">
-        <v>307</v>
-      </c>
-      <c r="E79" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F79" s="64"/>
+        <v>309</v>
+      </c>
+      <c r="E79" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" s="66"/>
     </row>
     <row r="80" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="60"/>
+      <c r="A80" s="62"/>
       <c r="B80" s="24"/>
       <c r="C80" s="22"/>
       <c r="D80" s="26" t="s">
-        <v>308</v>
-      </c>
-      <c r="E80" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F80" s="64"/>
+        <v>310</v>
+      </c>
+      <c r="E80" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" s="66"/>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="60"/>
+      <c r="A81" s="62"/>
       <c r="B81" s="24"/>
       <c r="C81" s="22"/>
       <c r="D81" s="26" t="s">
-        <v>309</v>
-      </c>
-      <c r="E81" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F81" s="64"/>
+        <v>311</v>
+      </c>
+      <c r="E81" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F81" s="66"/>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="60"/>
+      <c r="A82" s="62"/>
       <c r="B82" s="24"/>
       <c r="C82" s="22"/>
       <c r="D82" s="26" t="s">
-        <v>310</v>
-      </c>
-      <c r="E82" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F82" s="64"/>
+        <v>312</v>
+      </c>
+      <c r="E82" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" s="66"/>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="60"/>
+      <c r="A83" s="62"/>
       <c r="B83" s="24"/>
       <c r="C83" s="22"/>
       <c r="D83" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="E83" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F83" s="64"/>
+        <v>313</v>
+      </c>
+      <c r="E83" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F83" s="66"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="60"/>
+      <c r="A84" s="62"/>
       <c r="B84" s="24" t="n">
         <v>43</v>
       </c>
-      <c r="C84" s="61" t="s">
-        <v>312</v>
+      <c r="C84" s="63" t="s">
+        <v>314</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="E84" s="65" t="n">
+        <v>315</v>
+      </c>
+      <c r="E84" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F84" s="64"/>
+      <c r="F84" s="66"/>
     </row>
     <row r="85" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="60"/>
+      <c r="A85" s="62"/>
       <c r="B85" s="24" t="n">
         <v>44</v>
       </c>
-      <c r="C85" s="61" t="s">
-        <v>314</v>
+      <c r="C85" s="63" t="s">
+        <v>316</v>
       </c>
       <c r="D85" s="26"/>
-      <c r="E85" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F85" s="64"/>
+      <c r="E85" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" s="66"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="60" t="s">
-        <v>315</v>
+      <c r="A86" s="62" t="s">
+        <v>317</v>
       </c>
       <c r="B86" s="24" t="n">
         <v>45</v>
       </c>
-      <c r="C86" s="61" t="s">
-        <v>316</v>
+      <c r="C86" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="D86" s="26"/>
-      <c r="E86" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F86" s="64"/>
+      <c r="E86" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" s="66"/>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="60"/>
+      <c r="A87" s="62"/>
       <c r="B87" s="24" t="n">
         <v>46</v>
       </c>
-      <c r="C87" s="61" t="s">
-        <v>317</v>
+      <c r="C87" s="63" t="s">
+        <v>319</v>
       </c>
       <c r="D87" s="26"/>
-      <c r="E87" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F87" s="64"/>
+      <c r="E87" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" s="66"/>
     </row>
     <row r="88" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="60"/>
+      <c r="A88" s="62"/>
       <c r="B88" s="24" t="n">
         <v>47</v>
       </c>
-      <c r="C88" s="61" t="s">
-        <v>318</v>
+      <c r="C88" s="63" t="s">
+        <v>320</v>
       </c>
       <c r="D88" s="26"/>
-      <c r="E88" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F88" s="64"/>
+      <c r="E88" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" s="66"/>
     </row>
     <row r="89" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="60"/>
+      <c r="A89" s="62"/>
       <c r="B89" s="24" t="n">
         <v>48</v>
       </c>
-      <c r="C89" s="61" t="s">
-        <v>319</v>
+      <c r="C89" s="63" t="s">
+        <v>321</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>320</v>
-      </c>
-      <c r="E89" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F89" s="64"/>
+        <v>322</v>
+      </c>
+      <c r="E89" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F89" s="66"/>
     </row>
     <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="60"/>
+      <c r="A90" s="62"/>
       <c r="B90" s="24" t="n">
         <v>49</v>
       </c>
-      <c r="C90" s="61" t="s">
-        <v>321</v>
+      <c r="C90" s="63" t="s">
+        <v>323</v>
       </c>
       <c r="D90" s="26"/>
-      <c r="E90" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F90" s="64"/>
+      <c r="E90" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F90" s="66"/>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="60"/>
+      <c r="A91" s="62"/>
       <c r="B91" s="24" t="n">
         <v>50</v>
       </c>
-      <c r="C91" s="61" t="s">
-        <v>322</v>
+      <c r="C91" s="63" t="s">
+        <v>324</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>323</v>
-      </c>
-      <c r="E91" s="65" t="n">
+        <v>325</v>
+      </c>
+      <c r="E91" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="F91" s="64"/>
+      <c r="F91" s="66"/>
     </row>
     <row r="92" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="60" t="s">
-        <v>324</v>
+      <c r="A92" s="62" t="s">
+        <v>326</v>
       </c>
       <c r="B92" s="24" t="n">
         <v>51</v>
       </c>
-      <c r="C92" s="61" t="s">
-        <v>325</v>
+      <c r="C92" s="63" t="s">
+        <v>327</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>326</v>
-      </c>
-      <c r="E92" s="63" t="n">
+        <v>328</v>
+      </c>
+      <c r="E92" s="65" t="n">
         <v>4</v>
       </c>
-      <c r="F92" s="64"/>
+      <c r="F92" s="66"/>
     </row>
     <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="60"/>
+      <c r="A93" s="62"/>
       <c r="B93" s="24" t="n">
         <v>52</v>
       </c>
-      <c r="C93" s="61" t="s">
-        <v>327</v>
+      <c r="C93" s="63" t="s">
+        <v>329</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>328</v>
-      </c>
-      <c r="E93" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F93" s="64"/>
+        <v>330</v>
+      </c>
+      <c r="E93" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F93" s="66"/>
     </row>
     <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="60"/>
+      <c r="A94" s="62"/>
       <c r="B94" s="24" t="n">
         <v>53</v>
       </c>
-      <c r="C94" s="61" t="s">
-        <v>329</v>
+      <c r="C94" s="63" t="s">
+        <v>331</v>
       </c>
       <c r="D94" s="26"/>
-      <c r="E94" s="63" t="n">
+      <c r="E94" s="65" t="n">
         <v>2</v>
       </c>
-      <c r="F94" s="64"/>
+      <c r="F94" s="66"/>
     </row>
     <row r="95" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="60"/>
+      <c r="A95" s="62"/>
       <c r="B95" s="24" t="n">
         <v>54</v>
       </c>
-      <c r="C95" s="61" t="s">
-        <v>330</v>
+      <c r="C95" s="63" t="s">
+        <v>332</v>
       </c>
       <c r="D95" s="26"/>
-      <c r="E95" s="63" t="n">
+      <c r="E95" s="65" t="n">
         <v>4</v>
       </c>
-      <c r="F95" s="64"/>
+      <c r="F95" s="66"/>
     </row>
     <row r="96" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="60"/>
+      <c r="A96" s="62"/>
       <c r="B96" s="24" t="n">
         <v>55</v>
       </c>
-      <c r="C96" s="61" t="s">
-        <v>331</v>
+      <c r="C96" s="63" t="s">
+        <v>333</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>332</v>
-      </c>
-      <c r="E96" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F96" s="64"/>
+        <v>334</v>
+      </c>
+      <c r="E96" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" s="66"/>
     </row>
     <row r="97" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="60"/>
+      <c r="A97" s="62"/>
       <c r="B97" s="24" t="n">
         <v>56</v>
       </c>
-      <c r="C97" s="61" t="s">
-        <v>333</v>
+      <c r="C97" s="63" t="s">
+        <v>335</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="E97" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F97" s="64"/>
+        <v>336</v>
+      </c>
+      <c r="E97" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F97" s="66"/>
     </row>
     <row r="98" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="60"/>
+      <c r="A98" s="62"/>
       <c r="B98" s="24" t="n">
         <v>57</v>
       </c>
-      <c r="C98" s="61" t="s">
-        <v>335</v>
+      <c r="C98" s="63" t="s">
+        <v>337</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>336</v>
-      </c>
-      <c r="E98" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F98" s="64"/>
+        <v>338</v>
+      </c>
+      <c r="E98" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F98" s="66"/>
     </row>
     <row r="99" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="60"/>
+      <c r="A99" s="62"/>
       <c r="B99" s="24" t="n">
         <v>58</v>
       </c>
-      <c r="C99" s="61" t="s">
-        <v>337</v>
+      <c r="C99" s="63" t="s">
+        <v>339</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>338</v>
-      </c>
-      <c r="E99" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F99" s="64"/>
+        <v>340</v>
+      </c>
+      <c r="E99" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" s="66"/>
     </row>
     <row r="100" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="60"/>
+      <c r="A100" s="62"/>
       <c r="B100" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="C100" s="61" t="s">
-        <v>339</v>
+      <c r="C100" s="63" t="s">
+        <v>341</v>
       </c>
       <c r="D100" s="26"/>
-      <c r="E100" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F100" s="64"/>
+      <c r="E100" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F100" s="66"/>
     </row>
     <row r="101" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="60"/>
+      <c r="A101" s="62"/>
       <c r="B101" s="24" t="n">
         <v>60</v>
       </c>
-      <c r="C101" s="61" t="s">
-        <v>340</v>
+      <c r="C101" s="63" t="s">
+        <v>342</v>
       </c>
       <c r="D101" s="26"/>
-      <c r="E101" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F101" s="64"/>
+      <c r="E101" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F101" s="66"/>
     </row>
     <row r="102" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="60"/>
+      <c r="A102" s="62"/>
       <c r="B102" s="27" t="n">
         <v>61</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>342</v>
-      </c>
-      <c r="E102" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F102" s="64"/>
+        <v>344</v>
+      </c>
+      <c r="E102" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F102" s="66"/>
     </row>
     <row r="103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="60"/>
+      <c r="A103" s="62"/>
       <c r="B103" s="27"/>
       <c r="C103" s="22"/>
       <c r="D103" s="26" t="s">
-        <v>343</v>
-      </c>
-      <c r="E103" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F103" s="64"/>
+        <v>345</v>
+      </c>
+      <c r="E103" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F103" s="66"/>
     </row>
     <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="60"/>
+      <c r="A104" s="62"/>
       <c r="B104" s="27"/>
       <c r="C104" s="22"/>
       <c r="D104" s="26" t="s">
-        <v>344</v>
-      </c>
-      <c r="E104" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F104" s="64"/>
+        <v>346</v>
+      </c>
+      <c r="E104" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F104" s="66"/>
     </row>
     <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="60"/>
+      <c r="A105" s="62"/>
       <c r="B105" s="27"/>
       <c r="C105" s="22"/>
       <c r="D105" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="E105" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F105" s="64"/>
+        <v>293</v>
+      </c>
+      <c r="E105" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F105" s="66"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="60"/>
+      <c r="A106" s="62"/>
       <c r="B106" s="24" t="n">
         <v>62</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="E106" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F106" s="64"/>
+        <v>348</v>
+      </c>
+      <c r="E106" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F106" s="66"/>
     </row>
     <row r="107" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="60"/>
+      <c r="A107" s="62"/>
       <c r="B107" s="24"/>
       <c r="C107" s="22"/>
       <c r="D107" s="26" t="s">
-        <v>347</v>
-      </c>
-      <c r="E107" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F107" s="64"/>
+        <v>349</v>
+      </c>
+      <c r="E107" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F107" s="66"/>
     </row>
     <row r="108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="60"/>
+      <c r="A108" s="62"/>
       <c r="B108" s="24"/>
       <c r="C108" s="22"/>
       <c r="D108" s="26" t="s">
-        <v>348</v>
-      </c>
-      <c r="E108" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F108" s="64"/>
+        <v>350</v>
+      </c>
+      <c r="E108" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F108" s="66"/>
     </row>
     <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="60"/>
+      <c r="A109" s="62"/>
       <c r="B109" s="24"/>
       <c r="C109" s="22"/>
       <c r="D109" s="26" t="s">
-        <v>349</v>
-      </c>
-      <c r="E109" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F109" s="64"/>
+        <v>351</v>
+      </c>
+      <c r="E109" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F109" s="66"/>
     </row>
     <row r="110" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="60"/>
+      <c r="A110" s="62"/>
       <c r="B110" s="24"/>
       <c r="C110" s="22"/>
       <c r="D110" s="26" t="s">
-        <v>350</v>
-      </c>
-      <c r="E110" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F110" s="64"/>
+        <v>352</v>
+      </c>
+      <c r="E110" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F110" s="66"/>
     </row>
     <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="60"/>
+      <c r="A111" s="62"/>
       <c r="B111" s="24"/>
       <c r="C111" s="22"/>
       <c r="D111" s="26" t="s">
-        <v>351</v>
-      </c>
-      <c r="E111" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F111" s="64"/>
+        <v>353</v>
+      </c>
+      <c r="E111" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F111" s="66"/>
     </row>
     <row r="112" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="60"/>
+      <c r="A112" s="62"/>
       <c r="B112" s="24" t="n">
         <v>63</v>
       </c>
-      <c r="C112" s="61" t="s">
-        <v>352</v>
+      <c r="C112" s="63" t="s">
+        <v>354</v>
       </c>
       <c r="D112" s="26"/>
-      <c r="E112" s="63" t="n">
+      <c r="E112" s="65" t="n">
         <v>2</v>
       </c>
-      <c r="F112" s="64"/>
+      <c r="F112" s="66"/>
     </row>
     <row r="113" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="60"/>
+      <c r="A113" s="62"/>
       <c r="B113" s="24" t="n">
         <v>64</v>
       </c>
-      <c r="C113" s="61" t="s">
-        <v>353</v>
+      <c r="C113" s="63" t="s">
+        <v>355</v>
       </c>
       <c r="D113" s="26"/>
-      <c r="E113" s="63" t="n">
+      <c r="E113" s="65" t="n">
         <v>3</v>
       </c>
-      <c r="F113" s="64"/>
+      <c r="F113" s="66"/>
     </row>
     <row r="114" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="60"/>
+      <c r="A114" s="62"/>
       <c r="B114" s="24" t="n">
         <v>65</v>
       </c>
-      <c r="C114" s="61" t="s">
-        <v>354</v>
+      <c r="C114" s="63" t="s">
+        <v>356</v>
       </c>
       <c r="D114" s="26"/>
-      <c r="E114" s="63" t="n">
+      <c r="E114" s="65" t="n">
         <v>4</v>
       </c>
-      <c r="F114" s="64"/>
+      <c r="F114" s="66"/>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="60"/>
+      <c r="A115" s="62"/>
       <c r="B115" s="24" t="n">
         <v>66</v>
       </c>
-      <c r="C115" s="61" t="s">
-        <v>355</v>
+      <c r="C115" s="63" t="s">
+        <v>357</v>
       </c>
       <c r="D115" s="26"/>
-      <c r="E115" s="63" t="n">
+      <c r="E115" s="65" t="n">
         <v>2</v>
       </c>
-      <c r="F115" s="64"/>
+      <c r="F115" s="66"/>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="60"/>
+      <c r="A116" s="62"/>
       <c r="B116" s="24" t="n">
         <v>67</v>
       </c>
-      <c r="C116" s="61" t="s">
-        <v>356</v>
+      <c r="C116" s="63" t="s">
+        <v>358</v>
       </c>
       <c r="D116" s="26"/>
-      <c r="E116" s="63" t="n">
+      <c r="E116" s="65" t="n">
         <v>3</v>
       </c>
-      <c r="F116" s="64"/>
+      <c r="F116" s="66"/>
     </row>
     <row r="117" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="60"/>
+      <c r="A117" s="62"/>
       <c r="B117" s="24" t="n">
         <v>68</v>
       </c>
-      <c r="C117" s="61" t="s">
-        <v>357</v>
+      <c r="C117" s="63" t="s">
+        <v>359</v>
       </c>
       <c r="D117" s="26"/>
-      <c r="E117" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="F117" s="64"/>
+      <c r="E117" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F117" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -5864,13 +5890,13 @@
   </sheetPr>
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="66" width="50.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="68" width="50.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="96.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="15.14"/>
@@ -5879,189 +5905,189 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="67" t="s">
-        <v>358</v>
-      </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
+      <c r="B2" s="69" t="s">
+        <v>360</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68" t="s">
-        <v>359</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>360</v>
-      </c>
-      <c r="C3" s="57" t="s">
+      <c r="A3" s="70" t="s">
         <v>361</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="B3" s="58" t="s">
         <v>362</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="C3" s="59" t="s">
         <v>363</v>
       </c>
+      <c r="D3" s="71" t="s">
+        <v>364</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="71" t="s">
-        <v>364</v>
+      <c r="A4" s="73" t="s">
+        <v>366</v>
       </c>
       <c r="B4" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="61" t="s">
-        <v>364</v>
-      </c>
-      <c r="D4" s="72" t="n">
+      <c r="C4" s="63" t="s">
+        <v>366</v>
+      </c>
+      <c r="D4" s="74" t="n">
         <v>0.2</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="73" t="s">
-        <v>366</v>
-      </c>
-      <c r="B5" s="74" t="n">
+      <c r="A5" s="75" t="s">
+        <v>368</v>
+      </c>
+      <c r="B5" s="76" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="75" t="s">
-        <v>367</v>
-      </c>
-      <c r="D5" s="72" t="n">
+      <c r="C5" s="77" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5" s="74" t="n">
         <v>0.2</v>
       </c>
-      <c r="E5" s="76" t="n">
+      <c r="E5" s="78" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="73"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="75" t="s">
-        <v>368</v>
-      </c>
-      <c r="D6" s="77" t="n">
+      <c r="A6" s="75"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="77" t="s">
+        <v>370</v>
+      </c>
+      <c r="D6" s="79" t="n">
         <v>0.15</v>
       </c>
-      <c r="E6" s="76" t="n">
+      <c r="E6" s="78" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="78" t="s">
-        <v>369</v>
-      </c>
-      <c r="B7" s="74" t="n">
+      <c r="A7" s="80" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" s="76" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="75" t="s">
-        <v>370</v>
-      </c>
-      <c r="D7" s="77" t="n">
+      <c r="C7" s="77" t="s">
+        <v>372</v>
+      </c>
+      <c r="D7" s="79" t="n">
         <v>0.3</v>
       </c>
-      <c r="E7" s="76" t="n">
+      <c r="E7" s="78" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="78"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="75" t="s">
-        <v>371</v>
-      </c>
-      <c r="D8" s="77" t="n">
+      <c r="A8" s="80"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77" t="s">
+        <v>373</v>
+      </c>
+      <c r="D8" s="79" t="n">
         <v>0.15</v>
       </c>
-      <c r="E8" s="76" t="n">
+      <c r="E8" s="78" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="78"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="75" t="s">
-        <v>372</v>
-      </c>
-      <c r="D9" s="77" t="n">
+      <c r="A9" s="80"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="77" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="79" t="n">
         <v>0.15</v>
       </c>
-      <c r="E9" s="76" t="n">
+      <c r="E9" s="78" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="78" t="s">
-        <v>373</v>
-      </c>
-      <c r="B10" s="74" t="n">
+      <c r="A10" s="80" t="s">
+        <v>375</v>
+      </c>
+      <c r="B10" s="76" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="75" t="s">
-        <v>374</v>
-      </c>
-      <c r="D10" s="77" t="n">
+      <c r="C10" s="77" t="s">
+        <v>376</v>
+      </c>
+      <c r="D10" s="79" t="n">
         <v>-0.3</v>
       </c>
-      <c r="E10" s="76" t="n">
+      <c r="E10" s="78" t="n">
         <v>-0.3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="78"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="75" t="s">
-        <v>375</v>
-      </c>
-      <c r="D11" s="77" t="n">
+      <c r="A11" s="80"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="77" t="s">
+        <v>377</v>
+      </c>
+      <c r="D11" s="79" t="n">
         <v>-0.3</v>
       </c>
-      <c r="E11" s="76" t="n">
+      <c r="E11" s="78" t="n">
         <v>-0.3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="78" t="s">
-        <v>376</v>
-      </c>
-      <c r="B12" s="74" t="n">
+      <c r="A12" s="80" t="s">
+        <v>378</v>
+      </c>
+      <c r="B12" s="76" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="75" t="s">
-        <v>377</v>
-      </c>
-      <c r="D12" s="77" t="n">
+      <c r="C12" s="77" t="s">
+        <v>379</v>
+      </c>
+      <c r="D12" s="79" t="n">
         <v>0.3</v>
       </c>
-      <c r="E12" s="76" t="n">
+      <c r="E12" s="78" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="78"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="75" t="s">
-        <v>378</v>
-      </c>
-      <c r="D13" s="77" t="n">
+      <c r="A13" s="80"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="77" t="s">
+        <v>380</v>
+      </c>
+      <c r="D13" s="79" t="n">
         <v>0.4</v>
       </c>
-      <c r="E13" s="76" t="n">
+      <c r="E13" s="78" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="78"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="75" t="s">
-        <v>379</v>
-      </c>
-      <c r="D14" s="77" t="n">
+      <c r="A14" s="80"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="77" t="s">
+        <v>381</v>
+      </c>
+      <c r="D14" s="79" t="n">
         <v>0.4</v>
       </c>
-      <c r="E14" s="76" t="n">
+      <c r="E14" s="78" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -6100,131 +6126,131 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="79" width="4.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="80" width="31.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="80" width="50.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="81" width="138.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="79" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="79" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="81" width="4.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="82" width="31.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="82" width="50.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="83" width="138.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="81" width="8.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="81" width="8.53"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="82"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="84" t="s">
-        <v>380</v>
+      <c r="B2" s="84"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="86" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="85"/>
-      <c r="D3" s="86"/>
+      <c r="B3" s="87"/>
+      <c r="D3" s="88"/>
     </row>
     <row r="4" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="87" t="s">
-        <v>381</v>
-      </c>
-      <c r="C4" s="88" t="s">
-        <v>382</v>
-      </c>
-      <c r="D4" s="89" t="s">
+      <c r="B4" s="89" t="s">
         <v>383</v>
       </c>
+      <c r="C4" s="90" t="s">
+        <v>384</v>
+      </c>
+      <c r="D4" s="91" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="87" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="89" t="s">
-        <v>385</v>
+      <c r="B5" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="C5" s="90"/>
+      <c r="D5" s="91" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="87"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="89" t="s">
-        <v>386</v>
+      <c r="B6" s="89"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="91" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="87"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89" t="s">
-        <v>387</v>
+      <c r="B7" s="89"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="91" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="87"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="89" t="s">
-        <v>388</v>
+      <c r="B8" s="89"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="91" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="89" t="s">
-        <v>389</v>
+      <c r="B9" s="89"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="91" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="87"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="89" t="s">
-        <v>390</v>
+      <c r="B10" s="89"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="91" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="87" t="s">
-        <v>391</v>
-      </c>
-      <c r="C11" s="88" t="s">
-        <v>392</v>
-      </c>
-      <c r="D11" s="89" t="s">
+      <c r="B11" s="89" t="s">
         <v>393</v>
       </c>
+      <c r="C11" s="90" t="s">
+        <v>394</v>
+      </c>
+      <c r="D11" s="91" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="87" t="s">
-        <v>394</v>
-      </c>
-      <c r="C12" s="88" t="s">
-        <v>395</v>
-      </c>
-      <c r="D12" s="89" t="s">
+      <c r="B12" s="89" t="s">
         <v>396</v>
       </c>
+      <c r="C12" s="90" t="s">
+        <v>397</v>
+      </c>
+      <c r="D12" s="91" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="87" t="s">
-        <v>397</v>
-      </c>
-      <c r="C13" s="90" t="s">
-        <v>398</v>
-      </c>
-      <c r="D13" s="89" t="s">
+      <c r="B13" s="89" t="s">
         <v>399</v>
       </c>
+      <c r="C13" s="92" t="s">
+        <v>400</v>
+      </c>
+      <c r="D13" s="91" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="87" t="s">
-        <v>400</v>
-      </c>
-      <c r="C14" s="88"/>
-      <c r="D14" s="91" t="s">
-        <v>401</v>
-      </c>
-      <c r="E14" s="92"/>
-      <c r="F14" s="93"/>
+      <c r="B14" s="89" t="s">
+        <v>402</v>
+      </c>
+      <c r="C14" s="90"/>
+      <c r="D14" s="93" t="s">
+        <v>403</v>
+      </c>
+      <c r="E14" s="94"/>
+      <c r="F14" s="95"/>
     </row>
     <row r="15" customFormat="false" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="94"/>
-      <c r="C15" s="95" t="s">
-        <v>402</v>
-      </c>
-      <c r="D15" s="96" t="s">
-        <v>403</v>
+      <c r="B15" s="96"/>
+      <c r="C15" s="97" t="s">
+        <v>404</v>
+      </c>
+      <c r="D15" s="98" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#143 change order form manytomany fields rendering in css file.
</commit_message>
<xml_diff>
--- a/VOKSS прейскурант_ 2.xlsx
+++ b/VOKSS прейскурант_ 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="розподіл матеріалів (Fabric)" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
     <sheet name="формування ціни" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Ускладнюючі елементи (element_complexitygroup)'!$A$3:$F$117</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Ускладнюючі елементи (element_complexitygroup)'!$A$4:$F$118</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="407">
   <si>
     <t xml:space="preserve">Примерное распределение материалов по группам сложности в зависимости от трудоѐмкости обработки</t>
   </si>
@@ -584,6 +584,9 @@
     <t xml:space="preserve">ПЕРЕЧЕНЬ усложняющих элементов (сверх количества, учтѐнного в минимальной сложности)</t>
   </si>
   <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
     <t xml:space="preserve">додати можливість вибору!!!</t>
   </si>
   <si>
@@ -596,11 +599,53 @@
     <t xml:space="preserve">№</t>
   </si>
   <si>
-    <t xml:space="preserve">Наименование
-усложняющих эл-тов (group)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дополнительные характеристики усложняющих элементов (name)</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Наименование
+усложняющих эл-тов </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="16"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">(group)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Дополнительные характеристики усложняющих элементов </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="15"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">(name)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Кол-во
@@ -1304,7 +1349,7 @@
     <numFmt numFmtId="168" formatCode="D\-MMM"/>
     <numFmt numFmtId="169" formatCode="0%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1375,6 +1420,36 @@
       <charset val="204"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="16"/>
+      <color rgb="FFCE181E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <color rgb="FFCE181E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1408,8 +1483,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFED1C24"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FFF04E4D"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
@@ -1622,7 +1697,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="102">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1843,11 +1918,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1947,75 +2034,75 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2032,7 +2119,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFED1C24"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
@@ -2075,7 +2162,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFF04E4D"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -2098,7 +2185,7 @@
   </sheetPr>
   <dimension ref="B2:D35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4164,10 +4251,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A2:F117"/>
+  <dimension ref="A2:F118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4186,1692 +4273,1703 @@
         <v>178</v>
       </c>
       <c r="D2" s="54"/>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+    </row>
+    <row r="3" s="55" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="50"/>
+      <c r="C3" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="D3" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="58" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" s="61" customFormat="true" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="57" t="s">
+      <c r="F3" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="58" t="s">
+    </row>
+    <row r="4" s="64" customFormat="true" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="B4" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="C4" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="D4" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="E4" s="62" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="62" t="s">
+      <c r="F4" s="63" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="63" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="B5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="66" t="s">
         <v>189</v>
       </c>
-      <c r="E4" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="66" t="s">
+      <c r="D5" s="67" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="62"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="64" t="s">
+      <c r="E5" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="69" t="s">
         <v>191</v>
       </c>
-      <c r="E5" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="66" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="65"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="67" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="62"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="64" t="s">
+      <c r="E6" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="E6" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="66" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="65"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="67" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="62"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64" t="s">
+      <c r="E7" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="69" t="s">
         <v>195</v>
       </c>
-      <c r="E7" s="65" t="n">
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="65"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="67" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="66"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="62"/>
-      <c r="B8" s="24" t="n">
+      <c r="F8" s="69"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="65"/>
+      <c r="B9" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="63" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="C9" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="E8" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="66"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="62"/>
-      <c r="B9" s="24" t="n">
+      <c r="D9" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="69"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="65"/>
+      <c r="B10" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="63" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" s="26" t="s">
+      <c r="C10" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="E9" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="66"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="62"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="63"/>
       <c r="D10" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="E10" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="66"/>
+      <c r="E10" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="69"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="62"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="24"/>
-      <c r="C11" s="63"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="E11" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="66"/>
+      <c r="E11" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="69"/>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="62"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="24"/>
-      <c r="C12" s="63"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="E12" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="66"/>
+      <c r="E12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="69"/>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="62"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="24"/>
-      <c r="C13" s="63"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="66"/>
-    </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="62"/>
-      <c r="B14" s="24" t="n">
+      <c r="E13" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="69"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="65"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="E14" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="69"/>
+    </row>
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="65"/>
+      <c r="B15" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="63" t="s">
-        <v>204</v>
-      </c>
-      <c r="D14" s="26" t="s">
+      <c r="C15" s="66" t="s">
         <v>205</v>
       </c>
-      <c r="E14" s="65" t="n">
+      <c r="D15" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E15" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="66"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="62"/>
-      <c r="B15" s="24" t="n">
+      <c r="F15" s="69"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65"/>
+      <c r="B16" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="63" t="s">
-        <v>206</v>
-      </c>
-      <c r="D15" s="63" t="s">
+      <c r="C16" s="66" t="s">
         <v>207</v>
       </c>
-      <c r="E15" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="66"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="62"/>
-      <c r="B16" s="27" t="n">
+      <c r="D16" s="66" t="s">
+        <v>208</v>
+      </c>
+      <c r="E16" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="69"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="65"/>
+      <c r="B17" s="27" t="n">
         <v>6</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="D16" s="63" t="s">
+      <c r="C17" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="E16" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="66"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="62"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="66" t="s">
         <v>210</v>
       </c>
       <c r="E17" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="66"/>
+      <c r="F17" s="69"/>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="62"/>
+      <c r="A18" s="65"/>
       <c r="B18" s="27"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="66" t="s">
         <v>211</v>
       </c>
       <c r="E18" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="66"/>
-    </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="62" t="s">
+      <c r="F18" s="69"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="65"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="66" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="24" t="n">
+      <c r="E19" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="69"/>
+    </row>
+    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="24" t="n">
         <v>7</v>
       </c>
-      <c r="C19" s="63" t="s">
-        <v>213</v>
-      </c>
-      <c r="D19" s="63" t="s">
+      <c r="C20" s="66" t="s">
         <v>214</v>
       </c>
-      <c r="E19" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="66"/>
-    </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="62"/>
-      <c r="B20" s="24" t="n">
+      <c r="D20" s="66" t="s">
+        <v>215</v>
+      </c>
+      <c r="E20" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="69"/>
+    </row>
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="65"/>
+      <c r="B21" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="C20" s="63" t="s">
-        <v>215</v>
-      </c>
-      <c r="D20" s="63" t="s">
+      <c r="C21" s="66" t="s">
         <v>216</v>
       </c>
-      <c r="E20" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="66"/>
-    </row>
-    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="62"/>
-      <c r="B21" s="24" t="n">
+      <c r="D21" s="66" t="s">
+        <v>217</v>
+      </c>
+      <c r="E21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="69"/>
+    </row>
+    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="65"/>
+      <c r="B22" s="24" t="n">
         <v>9</v>
       </c>
-      <c r="C21" s="63" t="s">
-        <v>217</v>
-      </c>
-      <c r="D21" s="63" t="s">
+      <c r="C22" s="66" t="s">
         <v>218</v>
       </c>
-      <c r="E21" s="22" t="n">
+      <c r="D22" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="E22" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="F21" s="66"/>
-    </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="62"/>
-      <c r="B22" s="24" t="n">
+      <c r="F22" s="69"/>
+    </row>
+    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="65"/>
+      <c r="B23" s="24" t="n">
         <v>10</v>
       </c>
-      <c r="C22" s="63" t="s">
-        <v>219</v>
-      </c>
-      <c r="D22" s="63" t="s">
+      <c r="C23" s="66" t="s">
         <v>220</v>
       </c>
-      <c r="E22" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="66"/>
-    </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="62"/>
-      <c r="B23" s="24" t="n">
+      <c r="D23" s="66" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="69"/>
+    </row>
+    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="65"/>
+      <c r="B24" s="24" t="n">
         <v>11</v>
       </c>
-      <c r="C23" s="63" t="s">
-        <v>221</v>
-      </c>
-      <c r="D23" s="63" t="s">
+      <c r="C24" s="66" t="s">
         <v>222</v>
       </c>
-      <c r="E23" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="66"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="62"/>
-      <c r="B24" s="27" t="n">
+      <c r="D24" s="66" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="69"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="65"/>
+      <c r="B25" s="27" t="n">
         <v>12</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="D24" s="63" t="s">
+      <c r="C25" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="E24" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F24" s="66"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="62"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="63" t="s">
+      <c r="D25" s="66" t="s">
         <v>225</v>
       </c>
-      <c r="E25" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" s="66"/>
-    </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="62" t="s">
+      <c r="E25" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="69"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="65"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="66" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="24" t="n">
+      <c r="E26" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="69"/>
+    </row>
+    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="24" t="n">
         <v>13</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="D26" s="63" t="s">
+      <c r="C27" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="E26" s="65"/>
-      <c r="F26" s="66"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="62"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="63" t="s">
+      <c r="D27" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="E27" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" s="66"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="69"/>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="62"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="24"/>
       <c r="C28" s="22"/>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="66" t="s">
         <v>230</v>
       </c>
-      <c r="E28" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" s="66"/>
+      <c r="E28" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="62"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="24"/>
       <c r="C29" s="22"/>
       <c r="D29" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="E29" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F29" s="66"/>
+      <c r="E29" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="69"/>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="62"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="24"/>
       <c r="C30" s="22"/>
       <c r="D30" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="E30" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" s="66"/>
+      <c r="E30" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="69"/>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="62"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="24"/>
       <c r="C31" s="22"/>
       <c r="D31" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="E31" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" s="66"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="62"/>
+      <c r="E31" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="69"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="65"/>
       <c r="B32" s="24"/>
       <c r="C32" s="22"/>
       <c r="D32" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="E32" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" s="66"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="62"/>
-      <c r="B33" s="24" t="n">
+      <c r="E32" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" s="69"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="65"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="E33" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="69"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="65"/>
+      <c r="B34" s="24" t="n">
         <v>14</v>
       </c>
-      <c r="C33" s="63" t="s">
-        <v>235</v>
-      </c>
-      <c r="D33" s="26" t="s">
+      <c r="C34" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="E33" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" s="66"/>
-    </row>
-    <row r="34" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="62"/>
-      <c r="B34" s="24" t="n">
+      <c r="D34" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="E34" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="69"/>
+    </row>
+    <row r="35" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="65"/>
+      <c r="B35" s="24" t="n">
         <v>15</v>
       </c>
-      <c r="C34" s="63" t="s">
-        <v>237</v>
-      </c>
-      <c r="D34" s="26" t="s">
+      <c r="C35" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="E34" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="66"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="62"/>
-      <c r="B35" s="27" t="n">
+      <c r="D35" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="69"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="65"/>
+      <c r="B36" s="27" t="n">
         <v>16</v>
       </c>
-      <c r="C35" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="D35" s="26" t="s">
+      <c r="C36" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="E35" s="67" t="n">
-        <v>2</v>
-      </c>
-      <c r="F35" s="66"/>
-    </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="62"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="22"/>
       <c r="D36" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="E36" s="67" t="n">
+      <c r="E36" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F36" s="66"/>
-    </row>
-    <row r="37" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="62"/>
-      <c r="B37" s="24" t="n">
+      <c r="F36" s="69"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="65"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="E37" s="70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" s="69"/>
+    </row>
+    <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="65"/>
+      <c r="B38" s="24" t="n">
         <v>17</v>
       </c>
-      <c r="C37" s="63" t="s">
-        <v>242</v>
-      </c>
-      <c r="D37" s="26" t="s">
+      <c r="C38" s="66" t="s">
         <v>243</v>
       </c>
-      <c r="E37" s="67" t="n">
+      <c r="D38" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="E38" s="70" t="n">
         <v>4</v>
       </c>
-      <c r="F37" s="66"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="62" t="s">
-        <v>244</v>
-      </c>
-      <c r="B38" s="27" t="n">
+      <c r="F38" s="69"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="B39" s="27" t="n">
         <v>18</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="D38" s="26" t="s">
+      <c r="C39" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="E38" s="65"/>
-      <c r="F38" s="66"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="62"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="22"/>
       <c r="D39" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="E39" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" s="66"/>
-    </row>
-    <row r="40" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="62"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="69"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="65"/>
       <c r="B40" s="27"/>
       <c r="C40" s="22"/>
       <c r="D40" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="E40" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F40" s="66"/>
-    </row>
-    <row r="41" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="62"/>
-      <c r="B41" s="27" t="n">
+      <c r="E40" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="69"/>
+    </row>
+    <row r="41" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="65"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="E41" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="69"/>
+    </row>
+    <row r="42" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="65"/>
+      <c r="B42" s="27" t="n">
         <v>19</v>
       </c>
-      <c r="C41" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="D41" s="26" t="s">
+      <c r="C42" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="E41" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="66"/>
-    </row>
-    <row r="42" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="62"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="22"/>
       <c r="D42" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="E42" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" s="66"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="62"/>
-      <c r="B43" s="24" t="n">
+      <c r="E42" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="69"/>
+    </row>
+    <row r="43" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="65"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="E43" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="69"/>
+    </row>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="65"/>
+      <c r="B44" s="24" t="n">
         <v>20</v>
       </c>
-      <c r="C43" s="63" t="s">
-        <v>252</v>
-      </c>
-      <c r="D43" s="26" t="s">
+      <c r="C44" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E43" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" s="66"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="62"/>
-      <c r="B44" s="24" t="n">
+      <c r="D44" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="E44" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" s="69"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="65"/>
+      <c r="B45" s="24" t="n">
         <v>21</v>
       </c>
-      <c r="C44" s="63" t="s">
-        <v>254</v>
-      </c>
-      <c r="D44" s="26" t="s">
+      <c r="C45" s="66" t="s">
         <v>255</v>
       </c>
-      <c r="E44" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" s="66"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="62" t="s">
+      <c r="D45" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="B45" s="24" t="n">
+      <c r="E45" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="69"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="65" t="s">
+        <v>257</v>
+      </c>
+      <c r="B46" s="24" t="n">
         <v>22</v>
       </c>
-      <c r="C45" s="63" t="s">
-        <v>257</v>
-      </c>
-      <c r="D45" s="26" t="s">
+      <c r="C46" s="66" t="s">
         <v>258</v>
       </c>
-      <c r="E45" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" s="66"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="62"/>
-      <c r="B46" s="27" t="n">
+      <c r="D46" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="E46" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="69"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="65"/>
+      <c r="B47" s="27" t="n">
         <v>23</v>
       </c>
-      <c r="C46" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="D46" s="26" t="s">
+      <c r="C47" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="E46" s="67" t="n">
-        <v>2</v>
-      </c>
-      <c r="F46" s="66"/>
-    </row>
-    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="62"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="22"/>
       <c r="D47" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="E47" s="67" t="n">
+      <c r="E47" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F47" s="66"/>
+      <c r="F47" s="69"/>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="62"/>
+      <c r="A48" s="65"/>
       <c r="B48" s="27"/>
       <c r="C48" s="22"/>
       <c r="D48" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="E48" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" s="66"/>
+      <c r="E48" s="70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" s="69"/>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="62"/>
-      <c r="B49" s="24" t="n">
+      <c r="A49" s="65"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E49" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="69"/>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="65"/>
+      <c r="B50" s="24" t="n">
         <v>24</v>
       </c>
-      <c r="C49" s="63" t="s">
-        <v>263</v>
-      </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" s="66"/>
-    </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="62"/>
-      <c r="B50" s="24" t="n">
+      <c r="C50" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="D50" s="26"/>
+      <c r="E50" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="69"/>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="65"/>
+      <c r="B51" s="24" t="n">
         <v>25</v>
       </c>
-      <c r="C50" s="63" t="s">
-        <v>264</v>
-      </c>
-      <c r="D50" s="63" t="s">
+      <c r="C51" s="66" t="s">
         <v>265</v>
       </c>
-      <c r="E50" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" s="66"/>
-    </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="62"/>
-      <c r="B51" s="24" t="n">
+      <c r="D51" s="66" t="s">
+        <v>266</v>
+      </c>
+      <c r="E51" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" s="69"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="65"/>
+      <c r="B52" s="24" t="n">
         <v>26</v>
       </c>
-      <c r="C51" s="63" t="s">
-        <v>266</v>
-      </c>
-      <c r="D51" s="63" t="s">
+      <c r="C52" s="66" t="s">
         <v>267</v>
       </c>
-      <c r="E51" s="67" t="n">
+      <c r="D52" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="E52" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F51" s="66"/>
-    </row>
-    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="62"/>
-      <c r="B52" s="24" t="n">
+      <c r="F52" s="69"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="65"/>
+      <c r="B53" s="24" t="n">
         <v>27</v>
       </c>
-      <c r="C52" s="63" t="s">
+      <c r="C53" s="66" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" s="26"/>
+      <c r="E53" s="70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F53" s="69"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="65"/>
+      <c r="B54" s="24" t="n">
+        <v>28</v>
+      </c>
+      <c r="C54" s="66" t="s">
+        <v>270</v>
+      </c>
+      <c r="D54" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="D52" s="26"/>
-      <c r="E52" s="67" t="n">
+      <c r="E54" s="70" t="n">
+        <v>4</v>
+      </c>
+      <c r="F54" s="69"/>
+    </row>
+    <row r="55" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="65"/>
+      <c r="B55" s="24" t="n">
+        <v>29</v>
+      </c>
+      <c r="C55" s="66" t="s">
+        <v>271</v>
+      </c>
+      <c r="D55" s="26"/>
+      <c r="E55" s="70" t="n">
+        <v>4</v>
+      </c>
+      <c r="F55" s="69"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="65"/>
+      <c r="B56" s="24" t="n">
+        <v>30</v>
+      </c>
+      <c r="C56" s="66" t="s">
+        <v>272</v>
+      </c>
+      <c r="D56" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="E56" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" s="69"/>
+    </row>
+    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="65"/>
+      <c r="B57" s="24" t="n">
+        <v>31</v>
+      </c>
+      <c r="C57" s="66" t="s">
+        <v>274</v>
+      </c>
+      <c r="D57" s="66" t="s">
+        <v>275</v>
+      </c>
+      <c r="E57" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F52" s="66"/>
-    </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="62"/>
-      <c r="B53" s="24" t="n">
-        <v>28</v>
-      </c>
-      <c r="C53" s="63" t="s">
-        <v>269</v>
-      </c>
-      <c r="D53" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="E53" s="67" t="n">
-        <v>4</v>
-      </c>
-      <c r="F53" s="66"/>
-    </row>
-    <row r="54" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="62"/>
-      <c r="B54" s="24" t="n">
-        <v>29</v>
-      </c>
-      <c r="C54" s="63" t="s">
-        <v>270</v>
-      </c>
-      <c r="D54" s="26"/>
-      <c r="E54" s="67" t="n">
-        <v>4</v>
-      </c>
-      <c r="F54" s="66"/>
-    </row>
-    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="62"/>
-      <c r="B55" s="24" t="n">
-        <v>30</v>
-      </c>
-      <c r="C55" s="63" t="s">
-        <v>271</v>
-      </c>
-      <c r="D55" s="63" t="s">
-        <v>272</v>
-      </c>
-      <c r="E55" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F55" s="66"/>
-    </row>
-    <row r="56" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="62"/>
-      <c r="B56" s="24" t="n">
-        <v>31</v>
-      </c>
-      <c r="C56" s="63" t="s">
-        <v>273</v>
-      </c>
-      <c r="D56" s="63" t="s">
-        <v>274</v>
-      </c>
-      <c r="E56" s="67" t="n">
+      <c r="F57" s="69"/>
+    </row>
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="65"/>
+      <c r="B58" s="24" t="n">
+        <v>32</v>
+      </c>
+      <c r="C58" s="66" t="s">
+        <v>276</v>
+      </c>
+      <c r="D58" s="26"/>
+      <c r="E58" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" s="69"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="65"/>
+      <c r="B59" s="24" t="n">
+        <v>33</v>
+      </c>
+      <c r="C59" s="66" t="s">
+        <v>277</v>
+      </c>
+      <c r="D59" s="66" t="s">
+        <v>278</v>
+      </c>
+      <c r="E59" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F56" s="66"/>
-    </row>
-    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="62"/>
-      <c r="B57" s="24" t="n">
-        <v>32</v>
-      </c>
-      <c r="C57" s="63" t="s">
-        <v>275</v>
-      </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F57" s="66"/>
-    </row>
-    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="62"/>
-      <c r="B58" s="24" t="n">
-        <v>33</v>
-      </c>
-      <c r="C58" s="63" t="s">
-        <v>276</v>
-      </c>
-      <c r="D58" s="63" t="s">
-        <v>277</v>
-      </c>
-      <c r="E58" s="67" t="n">
-        <v>2</v>
-      </c>
-      <c r="F58" s="66"/>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="62" t="s">
-        <v>278</v>
-      </c>
-      <c r="B59" s="24" t="n">
+      <c r="F59" s="69"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="B60" s="24" t="n">
         <v>34</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="D59" s="63" t="s">
+      <c r="C60" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="E59" s="67"/>
-      <c r="F59" s="66"/>
-    </row>
-    <row r="60" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="62"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="63" t="s">
+      <c r="D60" s="66" t="s">
         <v>281</v>
       </c>
-      <c r="E60" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F60" s="66"/>
-    </row>
-    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="62"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="69"/>
+    </row>
+    <row r="61" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="65"/>
       <c r="B61" s="24"/>
       <c r="C61" s="22"/>
-      <c r="D61" s="63" t="s">
+      <c r="D61" s="66" t="s">
         <v>282</v>
       </c>
-      <c r="E61" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F61" s="66"/>
+      <c r="E61" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" s="69"/>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="62"/>
+      <c r="A62" s="65"/>
       <c r="B62" s="24"/>
       <c r="C62" s="22"/>
-      <c r="D62" s="63" t="s">
+      <c r="D62" s="66" t="s">
         <v>283</v>
       </c>
-      <c r="E62" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" s="66"/>
+      <c r="E62" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" s="69"/>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="62"/>
+      <c r="A63" s="65"/>
       <c r="B63" s="24"/>
       <c r="C63" s="22"/>
-      <c r="D63" s="63" t="s">
+      <c r="D63" s="66" t="s">
         <v>284</v>
       </c>
-      <c r="E63" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F63" s="66"/>
+      <c r="E63" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="69"/>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="62"/>
-      <c r="B64" s="24" t="n">
+      <c r="A64" s="65"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="66" t="s">
+        <v>285</v>
+      </c>
+      <c r="E64" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" s="69"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="65"/>
+      <c r="B65" s="24" t="n">
         <v>35</v>
       </c>
-      <c r="C64" s="63" t="s">
-        <v>285</v>
-      </c>
-      <c r="D64" s="63" t="s">
+      <c r="C65" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="E64" s="67" t="n">
+      <c r="D65" s="66" t="s">
+        <v>287</v>
+      </c>
+      <c r="E65" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F64" s="66"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="62"/>
-      <c r="B65" s="27" t="n">
+      <c r="F65" s="69"/>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="65"/>
+      <c r="B66" s="27" t="n">
         <v>36</v>
       </c>
-      <c r="C65" s="22" t="s">
-        <v>287</v>
-      </c>
-      <c r="D65" s="63" t="s">
+      <c r="C66" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="E65" s="65"/>
-      <c r="F65" s="66"/>
-    </row>
-    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="62"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="63" t="s">
+      <c r="D66" s="66" t="s">
         <v>289</v>
       </c>
-      <c r="E66" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" s="66"/>
-    </row>
-    <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="62"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="69"/>
+    </row>
+    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="65"/>
       <c r="B67" s="27"/>
       <c r="C67" s="22"/>
-      <c r="D67" s="63" t="s">
+      <c r="D67" s="66" t="s">
         <v>290</v>
       </c>
-      <c r="E67" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F67" s="66"/>
-    </row>
-    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="62"/>
-      <c r="B68" s="24" t="n">
+      <c r="E67" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" s="69"/>
+    </row>
+    <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="65"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="66" t="s">
+        <v>291</v>
+      </c>
+      <c r="E68" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" s="69"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="65"/>
+      <c r="B69" s="24" t="n">
         <v>37</v>
       </c>
-      <c r="C68" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="D68" s="63" t="s">
+      <c r="C69" s="66" t="s">
         <v>292</v>
       </c>
-      <c r="E68" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F68" s="66"/>
-    </row>
-    <row r="69" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="62" t="s">
+      <c r="D69" s="66" t="s">
         <v>293</v>
       </c>
-      <c r="B69" s="24" t="n">
+      <c r="E69" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" s="69"/>
+    </row>
+    <row r="70" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="B70" s="24" t="n">
         <v>38</v>
       </c>
-      <c r="C69" s="63" t="s">
-        <v>294</v>
-      </c>
-      <c r="D69" s="63" t="s">
+      <c r="C70" s="66" t="s">
         <v>295</v>
       </c>
-      <c r="E69" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F69" s="66"/>
-    </row>
-    <row r="70" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="62"/>
-      <c r="B70" s="24" t="n">
+      <c r="D70" s="66" t="s">
+        <v>296</v>
+      </c>
+      <c r="E70" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F70" s="69"/>
+    </row>
+    <row r="71" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="65"/>
+      <c r="B71" s="24" t="n">
         <v>39</v>
       </c>
-      <c r="C70" s="63" t="s">
-        <v>296</v>
-      </c>
-      <c r="D70" s="26" t="s">
+      <c r="C71" s="66" t="s">
         <v>297</v>
       </c>
-      <c r="E70" s="67" t="n">
+      <c r="D71" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="E71" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F70" s="66"/>
-    </row>
-    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="62"/>
-      <c r="B71" s="24" t="n">
+      <c r="F71" s="69"/>
+    </row>
+    <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="65"/>
+      <c r="B72" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="C71" s="63" t="s">
-        <v>298</v>
-      </c>
-      <c r="D71" s="63" t="s">
+      <c r="C72" s="66" t="s">
         <v>299</v>
       </c>
-      <c r="E71" s="67" t="n">
+      <c r="D72" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="E72" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F71" s="66"/>
-    </row>
-    <row r="72" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="62"/>
-      <c r="B72" s="24" t="n">
+      <c r="F72" s="69"/>
+    </row>
+    <row r="73" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="65"/>
+      <c r="B73" s="24" t="n">
         <v>41</v>
       </c>
-      <c r="C72" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="D72" s="63" t="s">
+      <c r="C73" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="E72" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F72" s="66"/>
-    </row>
-    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="62"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="63" t="s">
+      <c r="D73" s="66" t="s">
         <v>302</v>
       </c>
-      <c r="E73" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F73" s="66"/>
+      <c r="E73" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" s="69"/>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="62"/>
+      <c r="A74" s="65"/>
       <c r="B74" s="24"/>
       <c r="C74" s="22"/>
-      <c r="D74" s="63" t="s">
+      <c r="D74" s="66" t="s">
         <v>303</v>
       </c>
-      <c r="E74" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F74" s="66"/>
+      <c r="E74" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" s="69"/>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="62"/>
+      <c r="A75" s="65"/>
       <c r="B75" s="24"/>
       <c r="C75" s="22"/>
-      <c r="D75" s="63" t="s">
+      <c r="D75" s="66" t="s">
         <v>304</v>
       </c>
-      <c r="E75" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F75" s="66"/>
-    </row>
-    <row r="76" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="62"/>
+      <c r="E75" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" s="69"/>
+    </row>
+    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="65"/>
       <c r="B76" s="24"/>
       <c r="C76" s="22"/>
-      <c r="D76" s="63" t="s">
+      <c r="D76" s="66" t="s">
         <v>305</v>
       </c>
-      <c r="E76" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F76" s="66"/>
-    </row>
-    <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="62"/>
+      <c r="E76" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" s="69"/>
+    </row>
+    <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="65"/>
       <c r="B77" s="24"/>
       <c r="C77" s="22"/>
-      <c r="D77" s="63" t="s">
+      <c r="D77" s="66" t="s">
         <v>306</v>
       </c>
-      <c r="E77" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F77" s="66"/>
-    </row>
-    <row r="78" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="62"/>
-      <c r="B78" s="24" t="n">
+      <c r="E77" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" s="69"/>
+    </row>
+    <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="65"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="66" t="s">
+        <v>307</v>
+      </c>
+      <c r="E78" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" s="69"/>
+    </row>
+    <row r="79" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="65"/>
+      <c r="B79" s="24" t="n">
         <v>42</v>
       </c>
-      <c r="C78" s="22" t="s">
-        <v>307</v>
-      </c>
-      <c r="D78" s="26" t="s">
+      <c r="C79" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="E78" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F78" s="66"/>
-    </row>
-    <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="62"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="22"/>
       <c r="D79" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="E79" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F79" s="66"/>
-    </row>
-    <row r="80" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="62"/>
+      <c r="E79" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" s="69"/>
+    </row>
+    <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="65"/>
       <c r="B80" s="24"/>
       <c r="C80" s="22"/>
       <c r="D80" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="E80" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F80" s="66"/>
-    </row>
-    <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="62"/>
+      <c r="E80" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" s="69"/>
+    </row>
+    <row r="81" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="65"/>
       <c r="B81" s="24"/>
       <c r="C81" s="22"/>
       <c r="D81" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="E81" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F81" s="66"/>
+      <c r="E81" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F81" s="69"/>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="62"/>
+      <c r="A82" s="65"/>
       <c r="B82" s="24"/>
       <c r="C82" s="22"/>
       <c r="D82" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="E82" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F82" s="66"/>
+      <c r="E82" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" s="69"/>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="62"/>
+      <c r="A83" s="65"/>
       <c r="B83" s="24"/>
       <c r="C83" s="22"/>
       <c r="D83" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="E83" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F83" s="66"/>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="62"/>
-      <c r="B84" s="24" t="n">
+      <c r="E83" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F83" s="69"/>
+    </row>
+    <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="65"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="E84" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F84" s="69"/>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="65"/>
+      <c r="B85" s="24" t="n">
         <v>43</v>
       </c>
-      <c r="C84" s="63" t="s">
-        <v>314</v>
-      </c>
-      <c r="D84" s="26" t="s">
+      <c r="C85" s="66" t="s">
         <v>315</v>
       </c>
-      <c r="E84" s="67" t="n">
+      <c r="D85" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E85" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F84" s="66"/>
-    </row>
-    <row r="85" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="62"/>
-      <c r="B85" s="24" t="n">
+      <c r="F85" s="69"/>
+    </row>
+    <row r="86" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="65"/>
+      <c r="B86" s="24" t="n">
         <v>44</v>
       </c>
-      <c r="C85" s="63" t="s">
-        <v>316</v>
-      </c>
-      <c r="D85" s="26"/>
-      <c r="E85" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F85" s="66"/>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="62" t="s">
+      <c r="C86" s="66" t="s">
         <v>317</v>
       </c>
-      <c r="B86" s="24" t="n">
+      <c r="D86" s="26"/>
+      <c r="E86" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" s="69"/>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="65" t="s">
+        <v>318</v>
+      </c>
+      <c r="B87" s="24" t="n">
         <v>45</v>
       </c>
-      <c r="C86" s="63" t="s">
-        <v>318</v>
-      </c>
-      <c r="D86" s="26"/>
-      <c r="E86" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F86" s="66"/>
-    </row>
-    <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="62"/>
-      <c r="B87" s="24" t="n">
+      <c r="C87" s="66" t="s">
+        <v>319</v>
+      </c>
+      <c r="D87" s="26"/>
+      <c r="E87" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" s="69"/>
+    </row>
+    <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="65"/>
+      <c r="B88" s="24" t="n">
         <v>46</v>
       </c>
-      <c r="C87" s="63" t="s">
-        <v>319</v>
-      </c>
-      <c r="D87" s="26"/>
-      <c r="E87" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F87" s="66"/>
-    </row>
-    <row r="88" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="62"/>
-      <c r="B88" s="24" t="n">
+      <c r="C88" s="66" t="s">
+        <v>320</v>
+      </c>
+      <c r="D88" s="26"/>
+      <c r="E88" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" s="69"/>
+    </row>
+    <row r="89" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="65"/>
+      <c r="B89" s="24" t="n">
         <v>47</v>
       </c>
-      <c r="C88" s="63" t="s">
-        <v>320</v>
-      </c>
-      <c r="D88" s="26"/>
-      <c r="E88" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F88" s="66"/>
-    </row>
-    <row r="89" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="62"/>
-      <c r="B89" s="24" t="n">
+      <c r="C89" s="66" t="s">
+        <v>321</v>
+      </c>
+      <c r="D89" s="26"/>
+      <c r="E89" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F89" s="69"/>
+    </row>
+    <row r="90" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="65"/>
+      <c r="B90" s="24" t="n">
         <v>48</v>
       </c>
-      <c r="C89" s="63" t="s">
-        <v>321</v>
-      </c>
-      <c r="D89" s="26" t="s">
+      <c r="C90" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="E89" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F89" s="66"/>
-    </row>
-    <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="62"/>
-      <c r="B90" s="24" t="n">
+      <c r="D90" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="E90" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F90" s="69"/>
+    </row>
+    <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="65"/>
+      <c r="B91" s="24" t="n">
         <v>49</v>
       </c>
-      <c r="C90" s="63" t="s">
-        <v>323</v>
-      </c>
-      <c r="D90" s="26"/>
-      <c r="E90" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F90" s="66"/>
-    </row>
-    <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="62"/>
-      <c r="B91" s="24" t="n">
+      <c r="C91" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="D91" s="26"/>
+      <c r="E91" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F91" s="69"/>
+    </row>
+    <row r="92" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="65"/>
+      <c r="B92" s="24" t="n">
         <v>50</v>
       </c>
-      <c r="C91" s="63" t="s">
-        <v>324</v>
-      </c>
-      <c r="D91" s="26" t="s">
+      <c r="C92" s="66" t="s">
         <v>325</v>
       </c>
-      <c r="E91" s="67" t="n">
+      <c r="D92" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="E92" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="F91" s="66"/>
-    </row>
-    <row r="92" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="62" t="s">
-        <v>326</v>
-      </c>
-      <c r="B92" s="24" t="n">
+      <c r="F92" s="69"/>
+    </row>
+    <row r="93" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="65" t="s">
+        <v>327</v>
+      </c>
+      <c r="B93" s="24" t="n">
         <v>51</v>
       </c>
-      <c r="C92" s="63" t="s">
-        <v>327</v>
-      </c>
-      <c r="D92" s="26" t="s">
+      <c r="C93" s="66" t="s">
         <v>328</v>
       </c>
-      <c r="E92" s="65" t="n">
+      <c r="D93" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="E93" s="68" t="n">
         <v>4</v>
       </c>
-      <c r="F92" s="66"/>
-    </row>
-    <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="62"/>
-      <c r="B93" s="24" t="n">
+      <c r="F93" s="69"/>
+    </row>
+    <row r="94" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="65"/>
+      <c r="B94" s="24" t="n">
         <v>52</v>
       </c>
-      <c r="C93" s="63" t="s">
-        <v>329</v>
-      </c>
-      <c r="D93" s="26" t="s">
+      <c r="C94" s="66" t="s">
         <v>330</v>
       </c>
-      <c r="E93" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F93" s="66"/>
-    </row>
-    <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="62"/>
-      <c r="B94" s="24" t="n">
+      <c r="D94" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="E94" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F94" s="69"/>
+    </row>
+    <row r="95" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="65"/>
+      <c r="B95" s="24" t="n">
         <v>53</v>
       </c>
-      <c r="C94" s="63" t="s">
-        <v>331</v>
-      </c>
-      <c r="D94" s="26"/>
-      <c r="E94" s="65" t="n">
+      <c r="C95" s="66" t="s">
+        <v>332</v>
+      </c>
+      <c r="D95" s="26"/>
+      <c r="E95" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="F94" s="66"/>
-    </row>
-    <row r="95" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="62"/>
-      <c r="B95" s="24" t="n">
+      <c r="F95" s="69"/>
+    </row>
+    <row r="96" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="65"/>
+      <c r="B96" s="24" t="n">
         <v>54</v>
       </c>
-      <c r="C95" s="63" t="s">
-        <v>332</v>
-      </c>
-      <c r="D95" s="26"/>
-      <c r="E95" s="65" t="n">
+      <c r="C96" s="66" t="s">
+        <v>333</v>
+      </c>
+      <c r="D96" s="26"/>
+      <c r="E96" s="68" t="n">
         <v>4</v>
       </c>
-      <c r="F95" s="66"/>
-    </row>
-    <row r="96" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="62"/>
-      <c r="B96" s="24" t="n">
+      <c r="F96" s="69"/>
+    </row>
+    <row r="97" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="65"/>
+      <c r="B97" s="24" t="n">
         <v>55</v>
       </c>
-      <c r="C96" s="63" t="s">
-        <v>333</v>
-      </c>
-      <c r="D96" s="26" t="s">
+      <c r="C97" s="66" t="s">
         <v>334</v>
       </c>
-      <c r="E96" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F96" s="66"/>
-    </row>
-    <row r="97" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="62"/>
-      <c r="B97" s="24" t="n">
+      <c r="D97" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E97" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F97" s="69"/>
+    </row>
+    <row r="98" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="65"/>
+      <c r="B98" s="24" t="n">
         <v>56</v>
       </c>
-      <c r="C97" s="63" t="s">
-        <v>335</v>
-      </c>
-      <c r="D97" s="26" t="s">
+      <c r="C98" s="66" t="s">
         <v>336</v>
       </c>
-      <c r="E97" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F97" s="66"/>
-    </row>
-    <row r="98" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="62"/>
-      <c r="B98" s="24" t="n">
+      <c r="D98" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="E98" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F98" s="69"/>
+    </row>
+    <row r="99" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="65"/>
+      <c r="B99" s="24" t="n">
         <v>57</v>
       </c>
-      <c r="C98" s="63" t="s">
-        <v>337</v>
-      </c>
-      <c r="D98" s="26" t="s">
+      <c r="C99" s="66" t="s">
         <v>338</v>
       </c>
-      <c r="E98" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F98" s="66"/>
-    </row>
-    <row r="99" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="62"/>
-      <c r="B99" s="24" t="n">
+      <c r="D99" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="E99" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" s="69"/>
+    </row>
+    <row r="100" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="65"/>
+      <c r="B100" s="24" t="n">
         <v>58</v>
       </c>
-      <c r="C99" s="63" t="s">
-        <v>339</v>
-      </c>
-      <c r="D99" s="26" t="s">
+      <c r="C100" s="66" t="s">
         <v>340</v>
       </c>
-      <c r="E99" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F99" s="66"/>
-    </row>
-    <row r="100" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="62"/>
-      <c r="B100" s="24" t="n">
+      <c r="D100" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="E100" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F100" s="69"/>
+    </row>
+    <row r="101" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="65"/>
+      <c r="B101" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="C100" s="63" t="s">
-        <v>341</v>
-      </c>
-      <c r="D100" s="26"/>
-      <c r="E100" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F100" s="66"/>
-    </row>
-    <row r="101" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="62"/>
-      <c r="B101" s="24" t="n">
+      <c r="C101" s="66" t="s">
+        <v>342</v>
+      </c>
+      <c r="D101" s="26"/>
+      <c r="E101" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F101" s="69"/>
+    </row>
+    <row r="102" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="65"/>
+      <c r="B102" s="24" t="n">
         <v>60</v>
       </c>
-      <c r="C101" s="63" t="s">
-        <v>342</v>
-      </c>
-      <c r="D101" s="26"/>
-      <c r="E101" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F101" s="66"/>
-    </row>
-    <row r="102" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="62"/>
-      <c r="B102" s="27" t="n">
+      <c r="C102" s="66" t="s">
+        <v>343</v>
+      </c>
+      <c r="D102" s="26"/>
+      <c r="E102" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F102" s="69"/>
+    </row>
+    <row r="103" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="65"/>
+      <c r="B103" s="27" t="n">
         <v>61</v>
       </c>
-      <c r="C102" s="22" t="s">
-        <v>343</v>
-      </c>
-      <c r="D102" s="26" t="s">
+      <c r="C103" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="E102" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F102" s="66"/>
-    </row>
-    <row r="103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="62"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="22"/>
       <c r="D103" s="26" t="s">
         <v>345</v>
       </c>
-      <c r="E103" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F103" s="66"/>
+      <c r="E103" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F103" s="69"/>
     </row>
     <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="62"/>
+      <c r="A104" s="65"/>
       <c r="B104" s="27"/>
       <c r="C104" s="22"/>
       <c r="D104" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="E104" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F104" s="66"/>
+      <c r="E104" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F104" s="69"/>
     </row>
     <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="62"/>
+      <c r="A105" s="65"/>
       <c r="B105" s="27"/>
       <c r="C105" s="22"/>
       <c r="D105" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="E105" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F105" s="66"/>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="62"/>
-      <c r="B106" s="24" t="n">
+        <v>347</v>
+      </c>
+      <c r="E105" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F105" s="69"/>
+    </row>
+    <row r="106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="65"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="E106" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F106" s="69"/>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A107" s="65"/>
+      <c r="B107" s="24" t="n">
         <v>62</v>
       </c>
-      <c r="C106" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="D106" s="26" t="s">
+      <c r="C107" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="E106" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F106" s="66"/>
-    </row>
-    <row r="107" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="62"/>
-      <c r="B107" s="24"/>
-      <c r="C107" s="22"/>
       <c r="D107" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="E107" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F107" s="66"/>
+      <c r="E107" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F107" s="69"/>
     </row>
     <row r="108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="62"/>
+      <c r="A108" s="65"/>
       <c r="B108" s="24"/>
       <c r="C108" s="22"/>
       <c r="D108" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="E108" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F108" s="66"/>
+      <c r="E108" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F108" s="69"/>
     </row>
     <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="62"/>
+      <c r="A109" s="65"/>
       <c r="B109" s="24"/>
       <c r="C109" s="22"/>
       <c r="D109" s="26" t="s">
         <v>351</v>
       </c>
-      <c r="E109" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F109" s="66"/>
+      <c r="E109" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F109" s="69"/>
     </row>
     <row r="110" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="62"/>
+      <c r="A110" s="65"/>
       <c r="B110" s="24"/>
       <c r="C110" s="22"/>
       <c r="D110" s="26" t="s">
         <v>352</v>
       </c>
-      <c r="E110" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F110" s="66"/>
+      <c r="E110" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F110" s="69"/>
     </row>
     <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="62"/>
+      <c r="A111" s="65"/>
       <c r="B111" s="24"/>
       <c r="C111" s="22"/>
       <c r="D111" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="E111" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F111" s="66"/>
-    </row>
-    <row r="112" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="62"/>
-      <c r="B112" s="24" t="n">
+      <c r="E111" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F111" s="69"/>
+    </row>
+    <row r="112" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="65"/>
+      <c r="B112" s="24"/>
+      <c r="C112" s="22"/>
+      <c r="D112" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="E112" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F112" s="69"/>
+    </row>
+    <row r="113" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="65"/>
+      <c r="B113" s="24" t="n">
         <v>63</v>
       </c>
-      <c r="C112" s="63" t="s">
-        <v>354</v>
-      </c>
-      <c r="D112" s="26"/>
-      <c r="E112" s="65" t="n">
+      <c r="C113" s="66" t="s">
+        <v>355</v>
+      </c>
+      <c r="D113" s="26"/>
+      <c r="E113" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="F112" s="66"/>
-    </row>
-    <row r="113" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="62"/>
-      <c r="B113" s="24" t="n">
+      <c r="F113" s="69"/>
+    </row>
+    <row r="114" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="65"/>
+      <c r="B114" s="24" t="n">
         <v>64</v>
       </c>
-      <c r="C113" s="63" t="s">
-        <v>355</v>
-      </c>
-      <c r="D113" s="26"/>
-      <c r="E113" s="65" t="n">
+      <c r="C114" s="66" t="s">
+        <v>356</v>
+      </c>
+      <c r="D114" s="26"/>
+      <c r="E114" s="68" t="n">
         <v>3</v>
       </c>
-      <c r="F113" s="66"/>
-    </row>
-    <row r="114" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="62"/>
-      <c r="B114" s="24" t="n">
+      <c r="F114" s="69"/>
+    </row>
+    <row r="115" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="65"/>
+      <c r="B115" s="24" t="n">
         <v>65</v>
       </c>
-      <c r="C114" s="63" t="s">
-        <v>356</v>
-      </c>
-      <c r="D114" s="26"/>
-      <c r="E114" s="65" t="n">
+      <c r="C115" s="66" t="s">
+        <v>357</v>
+      </c>
+      <c r="D115" s="26"/>
+      <c r="E115" s="68" t="n">
         <v>4</v>
       </c>
-      <c r="F114" s="66"/>
-    </row>
-    <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="62"/>
-      <c r="B115" s="24" t="n">
+      <c r="F115" s="69"/>
+    </row>
+    <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="65"/>
+      <c r="B116" s="24" t="n">
         <v>66</v>
       </c>
-      <c r="C115" s="63" t="s">
-        <v>357</v>
-      </c>
-      <c r="D115" s="26"/>
-      <c r="E115" s="65" t="n">
+      <c r="C116" s="66" t="s">
+        <v>358</v>
+      </c>
+      <c r="D116" s="26"/>
+      <c r="E116" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="F115" s="66"/>
-    </row>
-    <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="62"/>
-      <c r="B116" s="24" t="n">
+      <c r="F116" s="69"/>
+    </row>
+    <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="65"/>
+      <c r="B117" s="24" t="n">
         <v>67</v>
       </c>
-      <c r="C116" s="63" t="s">
-        <v>358</v>
-      </c>
-      <c r="D116" s="26"/>
-      <c r="E116" s="65" t="n">
+      <c r="C117" s="66" t="s">
+        <v>359</v>
+      </c>
+      <c r="D117" s="26"/>
+      <c r="E117" s="68" t="n">
         <v>3</v>
       </c>
-      <c r="F116" s="66"/>
-    </row>
-    <row r="117" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="62"/>
-      <c r="B117" s="24" t="n">
+      <c r="F117" s="69"/>
+    </row>
+    <row r="118" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="65"/>
+      <c r="B118" s="24" t="n">
         <v>68</v>
       </c>
-      <c r="C117" s="63" t="s">
-        <v>359</v>
-      </c>
-      <c r="D117" s="26"/>
-      <c r="E117" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="F117" s="66"/>
+      <c r="C118" s="66" t="s">
+        <v>360</v>
+      </c>
+      <c r="D118" s="26"/>
+      <c r="E118" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F118" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A4:A18"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A38:A44"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A45:A58"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="A59:A68"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="A69:A85"/>
-    <mergeCell ref="B72:B77"/>
-    <mergeCell ref="C72:C77"/>
-    <mergeCell ref="B78:B83"/>
-    <mergeCell ref="C78:C83"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A92:A117"/>
-    <mergeCell ref="B102:B105"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="B106:B111"/>
-    <mergeCell ref="C106:C111"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A27:A38"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A46:A59"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A60:A69"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="A70:A86"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="C79:C84"/>
+    <mergeCell ref="A87:A92"/>
+    <mergeCell ref="A93:A118"/>
+    <mergeCell ref="B103:B106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="B107:B112"/>
+    <mergeCell ref="C107:C112"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5896,7 +5994,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="68" width="50.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="71" width="50.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="96.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="15.14"/>
@@ -5905,189 +6003,189 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="69" t="s">
-        <v>360</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
+      <c r="B2" s="72" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="70" t="s">
-        <v>361</v>
-      </c>
-      <c r="B3" s="58" t="s">
+      <c r="A3" s="73" t="s">
         <v>362</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="C3" s="62" t="s">
         <v>364</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="D3" s="74" t="s">
         <v>365</v>
       </c>
+      <c r="E3" s="75" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="73" t="s">
-        <v>366</v>
+      <c r="A4" s="76" t="s">
+        <v>367</v>
       </c>
       <c r="B4" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="63" t="s">
-        <v>366</v>
-      </c>
-      <c r="D4" s="74" t="n">
+      <c r="C4" s="66" t="s">
+        <v>367</v>
+      </c>
+      <c r="D4" s="77" t="n">
         <v>0.2</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="75" t="s">
-        <v>368</v>
-      </c>
-      <c r="B5" s="76" t="n">
+      <c r="A5" s="78" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" s="79" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="77" t="s">
-        <v>369</v>
-      </c>
-      <c r="D5" s="74" t="n">
+      <c r="C5" s="80" t="s">
+        <v>370</v>
+      </c>
+      <c r="D5" s="77" t="n">
         <v>0.2</v>
       </c>
-      <c r="E5" s="78" t="n">
+      <c r="E5" s="81" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="75"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="77" t="s">
-        <v>370</v>
-      </c>
-      <c r="D6" s="79" t="n">
+      <c r="A6" s="78"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="80" t="s">
+        <v>371</v>
+      </c>
+      <c r="D6" s="82" t="n">
         <v>0.15</v>
       </c>
-      <c r="E6" s="78" t="n">
+      <c r="E6" s="81" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="80" t="s">
-        <v>371</v>
-      </c>
-      <c r="B7" s="76" t="n">
+      <c r="A7" s="83" t="s">
+        <v>372</v>
+      </c>
+      <c r="B7" s="79" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="77" t="s">
-        <v>372</v>
-      </c>
-      <c r="D7" s="79" t="n">
+      <c r="C7" s="80" t="s">
+        <v>373</v>
+      </c>
+      <c r="D7" s="82" t="n">
         <v>0.3</v>
       </c>
-      <c r="E7" s="78" t="n">
+      <c r="E7" s="81" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="80"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77" t="s">
-        <v>373</v>
-      </c>
-      <c r="D8" s="79" t="n">
+      <c r="A8" s="83"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" s="82" t="n">
         <v>0.15</v>
       </c>
-      <c r="E8" s="78" t="n">
+      <c r="E8" s="81" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="80"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="77" t="s">
-        <v>374</v>
-      </c>
-      <c r="D9" s="79" t="n">
+      <c r="A9" s="83"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80" t="s">
+        <v>375</v>
+      </c>
+      <c r="D9" s="82" t="n">
         <v>0.15</v>
       </c>
-      <c r="E9" s="78" t="n">
+      <c r="E9" s="81" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="80" t="s">
-        <v>375</v>
-      </c>
-      <c r="B10" s="76" t="n">
+      <c r="A10" s="83" t="s">
+        <v>376</v>
+      </c>
+      <c r="B10" s="79" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="77" t="s">
-        <v>376</v>
-      </c>
-      <c r="D10" s="79" t="n">
+      <c r="C10" s="80" t="s">
+        <v>377</v>
+      </c>
+      <c r="D10" s="82" t="n">
         <v>-0.3</v>
       </c>
-      <c r="E10" s="78" t="n">
+      <c r="E10" s="81" t="n">
         <v>-0.3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="80"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="77" t="s">
-        <v>377</v>
-      </c>
-      <c r="D11" s="79" t="n">
+      <c r="A11" s="83"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80" t="s">
+        <v>378</v>
+      </c>
+      <c r="D11" s="82" t="n">
         <v>-0.3</v>
       </c>
-      <c r="E11" s="78" t="n">
+      <c r="E11" s="81" t="n">
         <v>-0.3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="80" t="s">
-        <v>378</v>
-      </c>
-      <c r="B12" s="76" t="n">
+      <c r="A12" s="83" t="s">
+        <v>379</v>
+      </c>
+      <c r="B12" s="79" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="77" t="s">
-        <v>379</v>
-      </c>
-      <c r="D12" s="79" t="n">
+      <c r="C12" s="80" t="s">
+        <v>380</v>
+      </c>
+      <c r="D12" s="82" t="n">
         <v>0.3</v>
       </c>
-      <c r="E12" s="78" t="n">
+      <c r="E12" s="81" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="80"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="77" t="s">
-        <v>380</v>
-      </c>
-      <c r="D13" s="79" t="n">
+      <c r="A13" s="83"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80" t="s">
+        <v>381</v>
+      </c>
+      <c r="D13" s="82" t="n">
         <v>0.4</v>
       </c>
-      <c r="E13" s="78" t="n">
+      <c r="E13" s="81" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="80"/>
-      <c r="B14" s="76"/>
-      <c r="C14" s="77" t="s">
-        <v>381</v>
-      </c>
-      <c r="D14" s="79" t="n">
+      <c r="A14" s="83"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="80" t="s">
+        <v>382</v>
+      </c>
+      <c r="D14" s="82" t="n">
         <v>0.4</v>
       </c>
-      <c r="E14" s="78" t="n">
+      <c r="E14" s="81" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -6126,131 +6224,131 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="81" width="4.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="82" width="31.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="82" width="50.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="83" width="138.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="81" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="81" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="84" width="4.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="85" width="31.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="85" width="50.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="86" width="138.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="84" width="8.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="84" width="8.53"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="84"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="86" t="s">
-        <v>382</v>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="89" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="87"/>
-      <c r="D3" s="88"/>
+      <c r="B3" s="90"/>
+      <c r="D3" s="91"/>
     </row>
     <row r="4" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="89" t="s">
-        <v>383</v>
-      </c>
-      <c r="C4" s="90" t="s">
+      <c r="B4" s="92" t="s">
         <v>384</v>
       </c>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="93" t="s">
         <v>385</v>
       </c>
+      <c r="D4" s="94" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="89" t="s">
-        <v>386</v>
-      </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91" t="s">
+      <c r="B5" s="92" t="s">
         <v>387</v>
       </c>
+      <c r="C5" s="93"/>
+      <c r="D5" s="94" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91" t="s">
-        <v>388</v>
+      <c r="B6" s="92"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="94" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="89"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="91" t="s">
-        <v>389</v>
+      <c r="B7" s="92"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="94" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="91" t="s">
-        <v>390</v>
+      <c r="B8" s="92"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="94" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="89"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="91" t="s">
-        <v>391</v>
+      <c r="B9" s="92"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="89"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="91" t="s">
-        <v>392</v>
+      <c r="B10" s="92"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="94" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="89" t="s">
-        <v>393</v>
-      </c>
-      <c r="C11" s="90" t="s">
+      <c r="B11" s="92" t="s">
         <v>394</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="C11" s="93" t="s">
         <v>395</v>
       </c>
+      <c r="D11" s="94" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="89" t="s">
-        <v>396</v>
-      </c>
-      <c r="C12" s="90" t="s">
+      <c r="B12" s="92" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="91" t="s">
+      <c r="C12" s="93" t="s">
         <v>398</v>
       </c>
+      <c r="D12" s="94" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="89" t="s">
-        <v>399</v>
-      </c>
-      <c r="C13" s="92" t="s">
+      <c r="B13" s="92" t="s">
         <v>400</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="C13" s="95" t="s">
         <v>401</v>
       </c>
+      <c r="D13" s="94" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="89" t="s">
-        <v>402</v>
-      </c>
-      <c r="C14" s="90"/>
-      <c r="D14" s="93" t="s">
+      <c r="B14" s="92" t="s">
         <v>403</v>
       </c>
-      <c r="E14" s="94"/>
-      <c r="F14" s="95"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="96" t="s">
+        <v>404</v>
+      </c>
+      <c r="E14" s="97"/>
+      <c r="F14" s="98"/>
     </row>
     <row r="15" customFormat="false" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="96"/>
-      <c r="C15" s="97" t="s">
-        <v>404</v>
-      </c>
-      <c r="D15" s="98" t="s">
+      <c r="B15" s="99"/>
+      <c r="C15" s="100" t="s">
         <v>405</v>
+      </c>
+      <c r="D15" s="101" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>